<commit_message>
V1.0 Matriz de historia de usuarios
</commit_message>
<xml_diff>
--- a/Primer Parcial/PREGAME/1. ELICITACION/1.3 Historias de usuario/G2_Matriz de Marco de Trabajo HU_V1.0.xlsx
+++ b/Primer Parcial/PREGAME/1. ELICITACION/1.3 Historias de usuario/G2_Matriz de Marco de Trabajo HU_V1.0.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DYNABOOK\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F084559B-5AA7-4D48-A053-805034770B2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{962D27B1-4907-4A03-8BBB-2BFEB523EF59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Formato descripción HU" sheetId="1" r:id="rId1"/>
-    <sheet name="Historia de Usuario" sheetId="2" r:id="rId2"/>
+    <sheet name="Historia de Usuario RF-02" sheetId="2" r:id="rId2"/>
     <sheet name="Historia de Usuario RF-03" sheetId="3" r:id="rId3"/>
+    <sheet name="Historia de Usuario RF-07" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="100">
   <si>
     <t>Matriz de Marco de Trabajo de HU</t>
   </si>
@@ -107,7 +108,7 @@
     <t>Ingresar correo → Validar credenciales → Acceder</t>
   </si>
   <si>
-    <t>Área TIC</t>
+    <t>Moisés Benalcázar</t>
   </si>
   <si>
     <t>Alta</t>
@@ -143,9 +144,6 @@
     <t>Elegir aula → Franja → Enviar solicitud</t>
   </si>
   <si>
-    <t>Coordinación Académica</t>
-  </si>
-  <si>
     <t>Solo permite una franja; si está disponible, registra solicitud.</t>
   </si>
   <si>
@@ -173,7 +171,7 @@
     <t>Algoritmo asigna proyector disponible según aula/horario al enviar solicitud.</t>
   </si>
   <si>
-    <t>Área TIC / Equipo Dev</t>
+    <t>Mateo Medranda</t>
   </si>
   <si>
     <t>Conflictivo</t>
@@ -206,9 +204,6 @@
     <t>Registrar entrega → Registrar devolución</t>
   </si>
   <si>
-    <t>Técnico AV</t>
-  </si>
-  <si>
     <t>Registra fecha/hora exacta; marca retrasos &gt;10 min.</t>
   </si>
   <si>
@@ -236,7 +231,7 @@
     <t>Elegir fecha → Aula → Consultar</t>
   </si>
   <si>
-    <t>Equipo de Análisis</t>
+    <t>Stefany Díaz</t>
   </si>
   <si>
     <t>Media</t>
@@ -270,9 +265,6 @@
   </si>
   <si>
     <t>Seleccionar filtros → Exportar PDF/Excel</t>
-  </si>
-  <si>
-    <t>Dirección Administrativa</t>
   </si>
   <si>
     <t>Reportes correctos según filtros.</t>
@@ -330,9 +322,6 @@
   </si>
   <si>
     <t>USUARIO</t>
-  </si>
-  <si>
-    <t>REQ001</t>
   </si>
   <si>
     <t>TIEMPO</t>
@@ -772,7 +761,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="92">
+  <cellXfs count="91">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -897,9 +886,6 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="14" fontId="16" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -981,7 +967,51 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="12">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC6EFCE"/>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFEB9C"/>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC6EFCE"/>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -1240,6 +1270,90 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>552450</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>266700</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1066800" cy="1162050"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="image1.jpg">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E6E77AD5-E76C-4712-B268-4699E5EF7E08}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr preferRelativeResize="0"/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10372725" y="1209675"/>
+          <a:ext cx="1066800" cy="1162050"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>266700</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1095375" cy="1162050"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="image2.jpg">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3D6FB54F-A0DB-4C77-B2A7-40EE927A3BE6}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{E6E77AD5-E76C-4712-B268-4699E5EF7E08}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr preferRelativeResize="0"/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8420100" y="1209675"/>
+          <a:ext cx="1095375" cy="1162050"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
@@ -1443,8 +1557,8 @@
   </sheetPr>
   <dimension ref="A1:Z1002"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="H5" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8:O8"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1"/>
@@ -1520,22 +1634,22 @@
     </row>
     <row r="3" spans="1:26" ht="45" customHeight="1">
       <c r="A3" s="2"/>
-      <c r="B3" s="63" t="s">
+      <c r="B3" s="62" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="64"/>
-      <c r="D3" s="64"/>
-      <c r="E3" s="64"/>
-      <c r="F3" s="64"/>
-      <c r="G3" s="64"/>
-      <c r="H3" s="64"/>
-      <c r="I3" s="64"/>
-      <c r="J3" s="64"/>
-      <c r="K3" s="64"/>
-      <c r="L3" s="64"/>
-      <c r="M3" s="64"/>
-      <c r="N3" s="64"/>
-      <c r="O3" s="65"/>
+      <c r="C3" s="63"/>
+      <c r="D3" s="63"/>
+      <c r="E3" s="63"/>
+      <c r="F3" s="63"/>
+      <c r="G3" s="63"/>
+      <c r="H3" s="63"/>
+      <c r="I3" s="63"/>
+      <c r="J3" s="63"/>
+      <c r="K3" s="63"/>
+      <c r="L3" s="63"/>
+      <c r="M3" s="63"/>
+      <c r="N3" s="63"/>
+      <c r="O3" s="64"/>
       <c r="P3" s="2"/>
       <c r="Q3" s="2"/>
       <c r="R3" s="2"/>
@@ -1652,7 +1766,7 @@
       <c r="G6" s="49" t="s">
         <v>20</v>
       </c>
-      <c r="H6" s="49" t="s">
+      <c r="H6" s="51" t="s">
         <v>21</v>
       </c>
       <c r="I6" s="49">
@@ -1709,7 +1823,7 @@
         <v>32</v>
       </c>
       <c r="H7" s="51" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="I7" s="51">
         <v>6</v>
@@ -1724,13 +1838,13 @@
         <v>23</v>
       </c>
       <c r="M7" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="N7" s="51" t="s">
         <v>34</v>
       </c>
-      <c r="N7" s="51" t="s">
+      <c r="O7" s="51" t="s">
         <v>35</v>
-      </c>
-      <c r="O7" s="51" t="s">
-        <v>36</v>
       </c>
       <c r="P7" s="42"/>
       <c r="Q7" s="2"/>
@@ -1747,46 +1861,46 @@
     <row r="8" spans="1:26" ht="75.75" customHeight="1">
       <c r="A8" s="2"/>
       <c r="B8" s="46" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" s="57" t="s">
         <v>37</v>
       </c>
-      <c r="C8" s="58" t="s">
+      <c r="D8" s="57" t="s">
         <v>38</v>
       </c>
-      <c r="D8" s="58" t="s">
+      <c r="E8" s="57" t="s">
         <v>39</v>
       </c>
-      <c r="E8" s="58" t="s">
+      <c r="F8" s="57" t="s">
         <v>40</v>
       </c>
-      <c r="F8" s="58" t="s">
+      <c r="G8" s="57" t="s">
         <v>41</v>
       </c>
-      <c r="G8" s="58" t="s">
+      <c r="H8" s="58" t="s">
         <v>42</v>
       </c>
-      <c r="H8" s="59" t="s">
+      <c r="I8" s="55">
+        <v>6</v>
+      </c>
+      <c r="J8" s="56">
+        <v>45856</v>
+      </c>
+      <c r="K8" s="59" t="s">
+        <v>22</v>
+      </c>
+      <c r="L8" s="60" t="s">
         <v>43</v>
       </c>
-      <c r="I8" s="56">
-        <v>6</v>
-      </c>
-      <c r="J8" s="57">
-        <v>45856</v>
-      </c>
-      <c r="K8" s="60" t="s">
-        <v>22</v>
-      </c>
-      <c r="L8" s="61" t="s">
+      <c r="M8" s="57" t="s">
         <v>44</v>
       </c>
-      <c r="M8" s="58" t="s">
+      <c r="N8" s="57" t="s">
         <v>45</v>
       </c>
-      <c r="N8" s="58" t="s">
+      <c r="O8" s="61" t="s">
         <v>46</v>
-      </c>
-      <c r="O8" s="62" t="s">
-        <v>47</v>
       </c>
       <c r="P8" s="42"/>
       <c r="Q8" s="2"/>
@@ -1803,30 +1917,30 @@
     <row r="9" spans="1:26" ht="75.75" customHeight="1">
       <c r="A9" s="42"/>
       <c r="B9" s="46" t="s">
+        <v>47</v>
+      </c>
+      <c r="C9" s="53" t="s">
         <v>48</v>
       </c>
-      <c r="C9" s="53" t="s">
+      <c r="D9" s="53" t="s">
         <v>49</v>
       </c>
-      <c r="D9" s="53" t="s">
+      <c r="E9" s="53" t="s">
         <v>50</v>
       </c>
-      <c r="E9" s="53" t="s">
+      <c r="F9" s="53" t="s">
         <v>51</v>
       </c>
-      <c r="F9" s="53" t="s">
+      <c r="G9" s="53" t="s">
         <v>52</v>
       </c>
-      <c r="G9" s="53" t="s">
-        <v>53</v>
-      </c>
-      <c r="H9" s="54" t="s">
-        <v>54</v>
+      <c r="H9" s="58" t="s">
+        <v>42</v>
       </c>
       <c r="I9" s="49">
         <v>5</v>
       </c>
-      <c r="J9" s="55">
+      <c r="J9" s="54">
         <v>45856</v>
       </c>
       <c r="K9" s="53" t="s">
@@ -1836,13 +1950,13 @@
         <v>23</v>
       </c>
       <c r="M9" s="53" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="N9" s="53" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="O9" s="53" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="P9" s="42"/>
       <c r="Q9" s="2"/>
@@ -1859,25 +1973,25 @@
     <row r="10" spans="1:26" ht="64.5" customHeight="1">
       <c r="A10" s="42"/>
       <c r="B10" s="46" t="s">
+        <v>56</v>
+      </c>
+      <c r="C10" s="49" t="s">
+        <v>57</v>
+      </c>
+      <c r="D10" s="49" t="s">
         <v>58</v>
       </c>
-      <c r="C10" s="49" t="s">
+      <c r="E10" s="49" t="s">
         <v>59</v>
       </c>
-      <c r="D10" s="49" t="s">
+      <c r="F10" s="49" t="s">
         <v>60</v>
       </c>
-      <c r="E10" s="49" t="s">
+      <c r="G10" s="49" t="s">
         <v>61</v>
       </c>
-      <c r="F10" s="49" t="s">
+      <c r="H10" s="49" t="s">
         <v>62</v>
-      </c>
-      <c r="G10" s="49" t="s">
-        <v>63</v>
-      </c>
-      <c r="H10" s="49" t="s">
-        <v>64</v>
       </c>
       <c r="I10" s="53">
         <v>4</v>
@@ -1886,19 +2000,19 @@
         <v>45857</v>
       </c>
       <c r="K10" s="49" t="s">
+        <v>63</v>
+      </c>
+      <c r="L10" s="49" t="s">
+        <v>64</v>
+      </c>
+      <c r="M10" s="49" t="s">
         <v>65</v>
       </c>
-      <c r="L10" s="49" t="s">
+      <c r="N10" s="49" t="s">
         <v>66</v>
       </c>
-      <c r="M10" s="49" t="s">
+      <c r="O10" s="49" t="s">
         <v>67</v>
-      </c>
-      <c r="N10" s="49" t="s">
-        <v>68</v>
-      </c>
-      <c r="O10" s="49" t="s">
-        <v>69</v>
       </c>
       <c r="P10" s="42"/>
       <c r="Q10" s="2"/>
@@ -1915,25 +2029,25 @@
     <row r="11" spans="1:26" ht="61.5" customHeight="1">
       <c r="A11" s="42"/>
       <c r="B11" s="46" t="s">
+        <v>68</v>
+      </c>
+      <c r="C11" s="49" t="s">
+        <v>69</v>
+      </c>
+      <c r="D11" s="49" t="s">
         <v>70</v>
       </c>
-      <c r="C11" s="49" t="s">
+      <c r="E11" s="49" t="s">
         <v>71</v>
       </c>
-      <c r="D11" s="49" t="s">
+      <c r="F11" s="49" t="s">
         <v>72</v>
       </c>
-      <c r="E11" s="49" t="s">
+      <c r="G11" s="49" t="s">
         <v>73</v>
       </c>
-      <c r="F11" s="49" t="s">
-        <v>74</v>
-      </c>
-      <c r="G11" s="49" t="s">
-        <v>75</v>
-      </c>
       <c r="H11" s="49" t="s">
-        <v>76</v>
+        <v>62</v>
       </c>
       <c r="I11" s="49">
         <v>8</v>
@@ -1942,19 +2056,19 @@
         <v>45860</v>
       </c>
       <c r="K11" s="49" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="L11" s="49" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="M11" s="49" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="N11" s="49" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="O11" s="49" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="P11" s="42"/>
       <c r="Q11" s="2"/>
@@ -1971,25 +2085,25 @@
     <row r="12" spans="1:26" ht="70.5" customHeight="1">
       <c r="A12" s="42"/>
       <c r="B12" s="46" t="s">
+        <v>77</v>
+      </c>
+      <c r="C12" s="49" t="s">
+        <v>78</v>
+      </c>
+      <c r="D12" s="49" t="s">
+        <v>79</v>
+      </c>
+      <c r="E12" s="49" t="s">
         <v>80</v>
       </c>
-      <c r="C12" s="49" t="s">
+      <c r="F12" s="49" t="s">
         <v>81</v>
       </c>
-      <c r="D12" s="49" t="s">
+      <c r="G12" s="49" t="s">
         <v>82</v>
       </c>
-      <c r="E12" s="49" t="s">
-        <v>83</v>
-      </c>
-      <c r="F12" s="49" t="s">
-        <v>84</v>
-      </c>
-      <c r="G12" s="49" t="s">
-        <v>85</v>
-      </c>
       <c r="H12" s="49" t="s">
-        <v>21</v>
+        <v>62</v>
       </c>
       <c r="I12" s="49">
         <v>12</v>
@@ -2001,16 +2115,16 @@
         <v>22</v>
       </c>
       <c r="L12" s="49" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="M12" s="49" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="N12" s="49" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="O12" s="49" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="P12" s="42"/>
       <c r="Q12" s="2"/>
@@ -2628,10 +2742,10 @@
       <c r="I34" s="3"/>
       <c r="J34" s="2"/>
       <c r="K34" s="4" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="L34" s="4" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="M34" s="2"/>
       <c r="N34" s="2"/>
@@ -2660,10 +2774,10 @@
       <c r="I35" s="3"/>
       <c r="J35" s="2"/>
       <c r="K35" s="4" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="L35" s="4" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="M35" s="2"/>
       <c r="N35" s="2"/>
@@ -2693,7 +2807,7 @@
       <c r="J36" s="2"/>
       <c r="K36" s="4"/>
       <c r="L36" s="4" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="M36" s="2"/>
       <c r="N36" s="2"/>
@@ -29803,7 +29917,9 @@
   </sheetPr>
   <dimension ref="A2:Z1000"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="R17" sqref="R17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -29928,23 +30044,23 @@
     </row>
     <row r="6" spans="1:26" ht="39.75" customHeight="1">
       <c r="A6" s="39"/>
-      <c r="B6" s="89" t="s">
-        <v>94</v>
+      <c r="B6" s="88" t="s">
+        <v>91</v>
       </c>
-      <c r="C6" s="64"/>
-      <c r="D6" s="64"/>
-      <c r="E6" s="64"/>
-      <c r="F6" s="64"/>
-      <c r="G6" s="64"/>
-      <c r="H6" s="64"/>
-      <c r="I6" s="64"/>
-      <c r="J6" s="64"/>
-      <c r="K6" s="64"/>
-      <c r="L6" s="64"/>
-      <c r="M6" s="64"/>
-      <c r="N6" s="64"/>
-      <c r="O6" s="64"/>
-      <c r="P6" s="65"/>
+      <c r="C6" s="63"/>
+      <c r="D6" s="63"/>
+      <c r="E6" s="63"/>
+      <c r="F6" s="63"/>
+      <c r="G6" s="63"/>
+      <c r="H6" s="63"/>
+      <c r="I6" s="63"/>
+      <c r="J6" s="63"/>
+      <c r="K6" s="63"/>
+      <c r="L6" s="63"/>
+      <c r="M6" s="63"/>
+      <c r="N6" s="63"/>
+      <c r="O6" s="63"/>
+      <c r="P6" s="64"/>
       <c r="Q6" s="39"/>
       <c r="R6" s="39"/>
       <c r="S6" s="39"/>
@@ -30019,15 +30135,15 @@
         <v>1</v>
       </c>
       <c r="D9" s="20"/>
-      <c r="E9" s="84" t="s">
-        <v>95</v>
+      <c r="E9" s="83" t="s">
+        <v>92</v>
       </c>
-      <c r="F9" s="65"/>
+      <c r="F9" s="64"/>
       <c r="G9" s="20"/>
-      <c r="H9" s="84" t="s">
+      <c r="H9" s="83" t="s">
         <v>11</v>
       </c>
-      <c r="I9" s="65"/>
+      <c r="I9" s="64"/>
       <c r="J9" s="21"/>
       <c r="K9" s="21"/>
       <c r="L9" s="21"/>
@@ -30050,20 +30166,20 @@
       <c r="A10" s="39"/>
       <c r="B10" s="37"/>
       <c r="C10" s="26" t="s">
-        <v>96</v>
+        <v>27</v>
       </c>
       <c r="D10" s="22"/>
-      <c r="E10" s="85" t="e">
+      <c r="E10" s="84" t="str">
         <f>VLOOKUP(C10,'Formato descripción HU'!B6:O23,5,0)</f>
-        <v>#N/A</v>
+        <v>Usuario solicitante</v>
       </c>
-      <c r="F10" s="65"/>
+      <c r="F10" s="64"/>
       <c r="G10" s="23"/>
-      <c r="H10" s="85" t="e">
+      <c r="H10" s="84" t="str">
         <f>VLOOKUP(C10,'Formato descripción HU'!B6:O23,11,0)</f>
-        <v>#N/A</v>
+        <v>No iniciado</v>
       </c>
-      <c r="I10" s="65"/>
+      <c r="I10" s="64"/>
       <c r="J10" s="23"/>
       <c r="K10" s="21"/>
       <c r="L10" s="21"/>
@@ -30114,18 +30230,18 @@
       <c r="A12" s="17"/>
       <c r="B12" s="37"/>
       <c r="C12" s="19" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="D12" s="22"/>
-      <c r="E12" s="84" t="s">
+      <c r="E12" s="83" t="s">
         <v>10</v>
       </c>
-      <c r="F12" s="65"/>
+      <c r="F12" s="64"/>
       <c r="G12" s="23"/>
-      <c r="H12" s="84" t="s">
-        <v>98</v>
+      <c r="H12" s="83" t="s">
+        <v>94</v>
       </c>
-      <c r="I12" s="65"/>
+      <c r="I12" s="64"/>
       <c r="J12" s="23"/>
       <c r="K12" s="25"/>
       <c r="L12" s="25"/>
@@ -30147,22 +30263,22 @@
     <row r="13" spans="1:26" ht="30" customHeight="1">
       <c r="A13" s="17"/>
       <c r="B13" s="37"/>
-      <c r="C13" s="26" t="e">
-        <f>VLOOKUP('Historia de Usuario'!C10,'Formato descripción HU'!B6:O23,8,0)</f>
-        <v>#N/A</v>
+      <c r="C13" s="26">
+        <f>VLOOKUP('Historia de Usuario RF-02'!C10,'Formato descripción HU'!B6:O23,8,0)</f>
+        <v>6</v>
       </c>
       <c r="D13" s="22"/>
-      <c r="E13" s="85" t="e">
+      <c r="E13" s="84" t="str">
         <f>VLOOKUP(C10,'Formato descripción HU'!B6:O23,10,0)</f>
-        <v>#N/A</v>
+        <v>Alta</v>
       </c>
-      <c r="F13" s="65"/>
+      <c r="F13" s="64"/>
       <c r="G13" s="23"/>
-      <c r="H13" s="85" t="e">
+      <c r="H13" s="84" t="str">
         <f>VLOOKUP(C10,'Formato descripción HU'!B6:O23,7,0)</f>
-        <v>#N/A</v>
+        <v>Moisés Benalcázar</v>
       </c>
-      <c r="I13" s="65"/>
+      <c r="I13" s="64"/>
       <c r="J13" s="23"/>
       <c r="K13" s="25"/>
       <c r="L13" s="25"/>
@@ -30212,34 +30328,34 @@
     <row r="15" spans="1:26" ht="19.5" customHeight="1">
       <c r="A15" s="17"/>
       <c r="B15" s="37"/>
-      <c r="C15" s="66" t="s">
-        <v>99</v>
+      <c r="C15" s="65" t="s">
+        <v>95</v>
       </c>
-      <c r="D15" s="91" t="e">
+      <c r="D15" s="90" t="str">
         <f>VLOOKUP(C10,'Formato descripción HU'!B6:O23,3,0)</f>
-        <v>#N/A</v>
+        <v>Seleccionar fecha, aula y franja</v>
       </c>
-      <c r="E15" s="71"/>
+      <c r="E15" s="70"/>
       <c r="F15" s="27"/>
-      <c r="G15" s="66" t="s">
-        <v>100</v>
+      <c r="G15" s="65" t="s">
+        <v>96</v>
       </c>
-      <c r="H15" s="91" t="e">
+      <c r="H15" s="90" t="str">
         <f>VLOOKUP(C10,'Formato descripción HU'!B6:O23,4,0)</f>
-        <v>#N/A</v>
+        <v>Reservar un proyector para clase</v>
       </c>
-      <c r="I15" s="70"/>
-      <c r="J15" s="71"/>
+      <c r="I15" s="69"/>
+      <c r="J15" s="70"/>
       <c r="K15" s="27"/>
-      <c r="L15" s="66" t="s">
-        <v>101</v>
+      <c r="L15" s="65" t="s">
+        <v>97</v>
       </c>
-      <c r="M15" s="69" t="e">
+      <c r="M15" s="68" t="str">
         <f>VLOOKUP(C10,'Formato descripción HU'!B6:O23,6,0)</f>
-        <v>#N/A</v>
+        <v>Elegir aula → Franja → Enviar solicitud</v>
       </c>
-      <c r="N15" s="70"/>
-      <c r="O15" s="71"/>
+      <c r="N15" s="69"/>
+      <c r="O15" s="70"/>
       <c r="P15" s="38"/>
       <c r="Q15" s="17"/>
       <c r="R15" s="17"/>
@@ -30255,19 +30371,19 @@
     <row r="16" spans="1:26" ht="19.5" customHeight="1">
       <c r="A16" s="17"/>
       <c r="B16" s="37"/>
-      <c r="C16" s="67"/>
-      <c r="D16" s="72"/>
-      <c r="E16" s="74"/>
+      <c r="C16" s="66"/>
+      <c r="D16" s="71"/>
+      <c r="E16" s="73"/>
       <c r="F16" s="27"/>
-      <c r="G16" s="67"/>
-      <c r="H16" s="72"/>
-      <c r="I16" s="73"/>
-      <c r="J16" s="74"/>
+      <c r="G16" s="66"/>
+      <c r="H16" s="71"/>
+      <c r="I16" s="72"/>
+      <c r="J16" s="73"/>
       <c r="K16" s="27"/>
-      <c r="L16" s="67"/>
-      <c r="M16" s="72"/>
-      <c r="N16" s="73"/>
-      <c r="O16" s="74"/>
+      <c r="L16" s="66"/>
+      <c r="M16" s="71"/>
+      <c r="N16" s="72"/>
+      <c r="O16" s="73"/>
       <c r="P16" s="38"/>
       <c r="Q16" s="17"/>
       <c r="R16" s="17"/>
@@ -30283,19 +30399,19 @@
     <row r="17" spans="1:26" ht="19.5" customHeight="1">
       <c r="A17" s="17"/>
       <c r="B17" s="37"/>
-      <c r="C17" s="68"/>
-      <c r="D17" s="75"/>
-      <c r="E17" s="77"/>
+      <c r="C17" s="67"/>
+      <c r="D17" s="74"/>
+      <c r="E17" s="76"/>
       <c r="F17" s="27"/>
-      <c r="G17" s="68"/>
-      <c r="H17" s="75"/>
-      <c r="I17" s="76"/>
-      <c r="J17" s="77"/>
+      <c r="G17" s="67"/>
+      <c r="H17" s="74"/>
+      <c r="I17" s="75"/>
+      <c r="J17" s="76"/>
       <c r="K17" s="27"/>
-      <c r="L17" s="68"/>
-      <c r="M17" s="75"/>
-      <c r="N17" s="76"/>
-      <c r="O17" s="77"/>
+      <c r="L17" s="67"/>
+      <c r="M17" s="74"/>
+      <c r="N17" s="75"/>
+      <c r="O17" s="76"/>
       <c r="P17" s="38"/>
       <c r="Q17" s="17"/>
       <c r="R17" s="17"/>
@@ -30339,24 +30455,24 @@
     <row r="19" spans="1:26" ht="19.5" customHeight="1">
       <c r="A19" s="39"/>
       <c r="B19" s="37"/>
-      <c r="C19" s="86" t="s">
-        <v>102</v>
+      <c r="C19" s="85" t="s">
+        <v>98</v>
       </c>
-      <c r="D19" s="71"/>
-      <c r="E19" s="78" t="e">
+      <c r="D19" s="70"/>
+      <c r="E19" s="77" t="str">
         <f>VLOOKUP(C10,'Formato descripción HU'!B6:O23,14,0)</f>
-        <v>#N/A</v>
+        <v>Solicitud de préstamo</v>
       </c>
-      <c r="F19" s="79"/>
-      <c r="G19" s="79"/>
-      <c r="H19" s="79"/>
-      <c r="I19" s="79"/>
-      <c r="J19" s="79"/>
-      <c r="K19" s="79"/>
-      <c r="L19" s="79"/>
-      <c r="M19" s="79"/>
-      <c r="N19" s="79"/>
-      <c r="O19" s="80"/>
+      <c r="F19" s="78"/>
+      <c r="G19" s="78"/>
+      <c r="H19" s="78"/>
+      <c r="I19" s="78"/>
+      <c r="J19" s="78"/>
+      <c r="K19" s="78"/>
+      <c r="L19" s="78"/>
+      <c r="M19" s="78"/>
+      <c r="N19" s="78"/>
+      <c r="O19" s="79"/>
       <c r="P19" s="38"/>
       <c r="Q19" s="17"/>
       <c r="R19" s="39"/>
@@ -30372,19 +30488,19 @@
     <row r="20" spans="1:26" ht="19.5" customHeight="1">
       <c r="A20" s="39"/>
       <c r="B20" s="37"/>
-      <c r="C20" s="75"/>
-      <c r="D20" s="77"/>
-      <c r="E20" s="81"/>
-      <c r="F20" s="82"/>
-      <c r="G20" s="82"/>
-      <c r="H20" s="82"/>
-      <c r="I20" s="82"/>
-      <c r="J20" s="82"/>
-      <c r="K20" s="82"/>
-      <c r="L20" s="82"/>
-      <c r="M20" s="82"/>
-      <c r="N20" s="82"/>
-      <c r="O20" s="83"/>
+      <c r="C20" s="74"/>
+      <c r="D20" s="76"/>
+      <c r="E20" s="80"/>
+      <c r="F20" s="81"/>
+      <c r="G20" s="81"/>
+      <c r="H20" s="81"/>
+      <c r="I20" s="81"/>
+      <c r="J20" s="81"/>
+      <c r="K20" s="81"/>
+      <c r="L20" s="81"/>
+      <c r="M20" s="81"/>
+      <c r="N20" s="81"/>
+      <c r="O20" s="82"/>
       <c r="P20" s="38"/>
       <c r="Q20" s="17"/>
       <c r="R20" s="39"/>
@@ -30428,29 +30544,29 @@
     <row r="22" spans="1:26" ht="19.5" customHeight="1">
       <c r="A22" s="17"/>
       <c r="B22" s="37"/>
-      <c r="C22" s="87" t="s">
-        <v>103</v>
+      <c r="C22" s="86" t="s">
+        <v>99</v>
       </c>
-      <c r="D22" s="71"/>
-      <c r="E22" s="88" t="e">
+      <c r="D22" s="70"/>
+      <c r="E22" s="87" t="str">
         <f>VLOOKUP(C10,'Formato descripción HU'!B6:O23,12,0)</f>
-        <v>#N/A</v>
+        <v>Solo permite una franja; si está disponible, registra solicitud.</v>
       </c>
-      <c r="F22" s="70"/>
-      <c r="G22" s="70"/>
-      <c r="H22" s="71"/>
+      <c r="F22" s="69"/>
+      <c r="G22" s="69"/>
+      <c r="H22" s="70"/>
       <c r="I22" s="21"/>
-      <c r="J22" s="87" t="s">
+      <c r="J22" s="86" t="s">
         <v>13</v>
       </c>
-      <c r="K22" s="71"/>
-      <c r="L22" s="90" t="e">
+      <c r="K22" s="70"/>
+      <c r="L22" s="89" t="str">
         <f>VLOOKUP(C10,'Formato descripción HU'!B6:O23,13,0)</f>
-        <v>#N/A</v>
+        <v>Validación de horario</v>
       </c>
-      <c r="M22" s="70"/>
-      <c r="N22" s="70"/>
-      <c r="O22" s="71"/>
+      <c r="M22" s="69"/>
+      <c r="N22" s="69"/>
+      <c r="O22" s="70"/>
       <c r="P22" s="38"/>
       <c r="Q22" s="17"/>
       <c r="R22" s="17"/>
@@ -30466,19 +30582,19 @@
     <row r="23" spans="1:26" ht="19.5" customHeight="1">
       <c r="A23" s="17"/>
       <c r="B23" s="37"/>
-      <c r="C23" s="72"/>
-      <c r="D23" s="74"/>
-      <c r="E23" s="72"/>
-      <c r="F23" s="73"/>
-      <c r="G23" s="73"/>
-      <c r="H23" s="74"/>
+      <c r="C23" s="71"/>
+      <c r="D23" s="73"/>
+      <c r="E23" s="71"/>
+      <c r="F23" s="72"/>
+      <c r="G23" s="72"/>
+      <c r="H23" s="73"/>
       <c r="I23" s="21"/>
-      <c r="J23" s="72"/>
-      <c r="K23" s="74"/>
-      <c r="L23" s="72"/>
-      <c r="M23" s="73"/>
-      <c r="N23" s="73"/>
-      <c r="O23" s="74"/>
+      <c r="J23" s="71"/>
+      <c r="K23" s="73"/>
+      <c r="L23" s="71"/>
+      <c r="M23" s="72"/>
+      <c r="N23" s="72"/>
+      <c r="O23" s="73"/>
       <c r="P23" s="38"/>
       <c r="Q23" s="17"/>
       <c r="R23" s="17"/>
@@ -30494,19 +30610,19 @@
     <row r="24" spans="1:26" ht="19.5" customHeight="1">
       <c r="A24" s="17"/>
       <c r="B24" s="37"/>
-      <c r="C24" s="75"/>
-      <c r="D24" s="77"/>
-      <c r="E24" s="75"/>
-      <c r="F24" s="76"/>
-      <c r="G24" s="76"/>
-      <c r="H24" s="77"/>
+      <c r="C24" s="74"/>
+      <c r="D24" s="76"/>
+      <c r="E24" s="74"/>
+      <c r="F24" s="75"/>
+      <c r="G24" s="75"/>
+      <c r="H24" s="76"/>
       <c r="I24" s="21"/>
-      <c r="J24" s="75"/>
-      <c r="K24" s="77"/>
-      <c r="L24" s="75"/>
-      <c r="M24" s="76"/>
-      <c r="N24" s="76"/>
-      <c r="O24" s="77"/>
+      <c r="J24" s="74"/>
+      <c r="K24" s="76"/>
+      <c r="L24" s="74"/>
+      <c r="M24" s="75"/>
+      <c r="N24" s="75"/>
+      <c r="O24" s="76"/>
       <c r="P24" s="38"/>
       <c r="Q24" s="17"/>
       <c r="R24" s="17"/>
@@ -32408,22 +32524,22 @@
     <mergeCell ref="E13:F13"/>
   </mergeCells>
   <conditionalFormatting sqref="H10:I11">
-    <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="1" operator="equal">
       <formula>"Atrasado"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H10:I11">
-    <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="2" operator="equal">
       <formula>"Terminado"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H10:I11">
-    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="3" operator="equal">
       <formula>"En proceso"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H10:I11">
-    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="4" operator="equal">
       <formula>"No Iniciado"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -32453,7 +32569,9 @@
   </sheetPr>
   <dimension ref="A2:Z1000"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="S12" sqref="S12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -32480,23 +32598,23 @@
       <c r="F5" s="16"/>
     </row>
     <row r="6" spans="1:26" ht="39.75" customHeight="1">
-      <c r="B6" s="89" t="s">
-        <v>94</v>
+      <c r="B6" s="88" t="s">
+        <v>91</v>
       </c>
-      <c r="C6" s="64"/>
-      <c r="D6" s="64"/>
-      <c r="E6" s="64"/>
-      <c r="F6" s="64"/>
-      <c r="G6" s="64"/>
-      <c r="H6" s="64"/>
-      <c r="I6" s="64"/>
-      <c r="J6" s="64"/>
-      <c r="K6" s="64"/>
-      <c r="L6" s="64"/>
-      <c r="M6" s="64"/>
-      <c r="N6" s="64"/>
-      <c r="O6" s="64"/>
-      <c r="P6" s="65"/>
+      <c r="C6" s="63"/>
+      <c r="D6" s="63"/>
+      <c r="E6" s="63"/>
+      <c r="F6" s="63"/>
+      <c r="G6" s="63"/>
+      <c r="H6" s="63"/>
+      <c r="I6" s="63"/>
+      <c r="J6" s="63"/>
+      <c r="K6" s="63"/>
+      <c r="L6" s="63"/>
+      <c r="M6" s="63"/>
+      <c r="N6" s="63"/>
+      <c r="O6" s="63"/>
+      <c r="P6" s="64"/>
     </row>
     <row r="7" spans="1:26" ht="9.75" customHeight="1">
       <c r="A7" s="17"/>
@@ -32550,15 +32668,15 @@
         <v>1</v>
       </c>
       <c r="D9" s="20"/>
-      <c r="E9" s="84" t="s">
-        <v>95</v>
+      <c r="E9" s="83" t="s">
+        <v>92</v>
       </c>
-      <c r="F9" s="65"/>
+      <c r="F9" s="64"/>
       <c r="G9" s="20"/>
-      <c r="H9" s="84" t="s">
+      <c r="H9" s="83" t="s">
         <v>11</v>
       </c>
-      <c r="I9" s="65"/>
+      <c r="I9" s="64"/>
       <c r="J9" s="21"/>
       <c r="K9" s="21"/>
       <c r="L9" s="21"/>
@@ -32571,20 +32689,20 @@
     <row r="10" spans="1:26" ht="30" customHeight="1">
       <c r="B10" s="37"/>
       <c r="C10" s="26" t="s">
-        <v>96</v>
+        <v>36</v>
       </c>
       <c r="D10" s="22"/>
-      <c r="E10" s="85" t="e">
+      <c r="E10" s="84" t="str">
         <f>VLOOKUP(C10,'Formato descripción HU'!B6:O23,5,0)</f>
-        <v>#N/A</v>
+        <v>Personal Técnico / Sistema.</v>
       </c>
-      <c r="F10" s="65"/>
+      <c r="F10" s="64"/>
       <c r="G10" s="23"/>
-      <c r="H10" s="85" t="e">
+      <c r="H10" s="84" t="str">
         <f>VLOOKUP(C10,'Formato descripción HU'!B6:O23,11,0)</f>
-        <v>#N/A</v>
+        <v>Conflictivo</v>
       </c>
-      <c r="I10" s="65"/>
+      <c r="I10" s="64"/>
       <c r="J10" s="23"/>
       <c r="K10" s="21"/>
       <c r="L10" s="21"/>
@@ -32626,18 +32744,18 @@
       <c r="A12" s="17"/>
       <c r="B12" s="37"/>
       <c r="C12" s="19" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="D12" s="22"/>
-      <c r="E12" s="84" t="s">
+      <c r="E12" s="83" t="s">
         <v>10</v>
       </c>
-      <c r="F12" s="65"/>
+      <c r="F12" s="64"/>
       <c r="G12" s="23"/>
-      <c r="H12" s="84" t="s">
-        <v>98</v>
+      <c r="H12" s="83" t="s">
+        <v>94</v>
       </c>
-      <c r="I12" s="65"/>
+      <c r="I12" s="64"/>
       <c r="J12" s="23"/>
       <c r="K12" s="25"/>
       <c r="L12" s="25"/>
@@ -32659,22 +32777,22 @@
     <row r="13" spans="1:26" ht="30" customHeight="1">
       <c r="A13" s="17"/>
       <c r="B13" s="37"/>
-      <c r="C13" s="26" t="e">
+      <c r="C13" s="26">
         <f>VLOOKUP('Historia de Usuario RF-03'!C10,'Formato descripción HU'!B6:O23,8,0)</f>
-        <v>#N/A</v>
+        <v>6</v>
       </c>
       <c r="D13" s="22"/>
-      <c r="E13" s="85" t="e">
+      <c r="E13" s="84" t="str">
         <f>VLOOKUP(C10,'Formato descripción HU'!B6:O23,10,0)</f>
-        <v>#N/A</v>
+        <v>Alta</v>
       </c>
-      <c r="F13" s="65"/>
+      <c r="F13" s="64"/>
       <c r="G13" s="23"/>
-      <c r="H13" s="85" t="e">
+      <c r="H13" s="84" t="str">
         <f>VLOOKUP(C10,'Formato descripción HU'!B6:O23,7,0)</f>
-        <v>#N/A</v>
+        <v>Mateo Medranda</v>
       </c>
-      <c r="I13" s="65"/>
+      <c r="I13" s="64"/>
       <c r="J13" s="23"/>
       <c r="K13" s="25"/>
       <c r="L13" s="25"/>
@@ -32724,34 +32842,34 @@
     <row r="15" spans="1:26" ht="19.5" customHeight="1">
       <c r="A15" s="17"/>
       <c r="B15" s="37"/>
-      <c r="C15" s="66" t="s">
-        <v>99</v>
+      <c r="C15" s="65" t="s">
+        <v>95</v>
       </c>
-      <c r="D15" s="91" t="e">
+      <c r="D15" s="90" t="str">
         <f>VLOOKUP(C10,'Formato descripción HU'!B6:O23,3,0)</f>
-        <v>#N/A</v>
+        <v>Asignación automática de equipos disponibles.</v>
       </c>
-      <c r="E15" s="71"/>
+      <c r="E15" s="70"/>
       <c r="F15" s="27"/>
-      <c r="G15" s="66" t="s">
-        <v>100</v>
+      <c r="G15" s="65" t="s">
+        <v>96</v>
       </c>
-      <c r="H15" s="91" t="e">
+      <c r="H15" s="90" t="str">
         <f>VLOOKUP(C10,'Formato descripción HU'!B6:O23,4,0)</f>
-        <v>#N/A</v>
+        <v>Agilizar el préstamo y bloquear stock sin intervención técnica.</v>
       </c>
-      <c r="I15" s="70"/>
-      <c r="J15" s="71"/>
+      <c r="I15" s="69"/>
+      <c r="J15" s="70"/>
       <c r="K15" s="27"/>
-      <c r="L15" s="66" t="s">
-        <v>101</v>
+      <c r="L15" s="65" t="s">
+        <v>97</v>
       </c>
-      <c r="M15" s="69" t="e">
+      <c r="M15" s="68" t="str">
         <f>VLOOKUP(C10,'Formato descripción HU'!B6:O23,6,0)</f>
-        <v>#N/A</v>
+        <v>Algoritmo asigna proyector disponible según aula/horario al enviar solicitud.</v>
       </c>
-      <c r="N15" s="70"/>
-      <c r="O15" s="71"/>
+      <c r="N15" s="69"/>
+      <c r="O15" s="70"/>
       <c r="P15" s="38"/>
       <c r="Q15" s="17"/>
       <c r="R15" s="17"/>
@@ -32767,19 +32885,19 @@
     <row r="16" spans="1:26" ht="19.5" customHeight="1">
       <c r="A16" s="17"/>
       <c r="B16" s="37"/>
-      <c r="C16" s="67"/>
-      <c r="D16" s="72"/>
-      <c r="E16" s="74"/>
+      <c r="C16" s="66"/>
+      <c r="D16" s="71"/>
+      <c r="E16" s="73"/>
       <c r="F16" s="27"/>
-      <c r="G16" s="67"/>
-      <c r="H16" s="72"/>
-      <c r="I16" s="73"/>
-      <c r="J16" s="74"/>
+      <c r="G16" s="66"/>
+      <c r="H16" s="71"/>
+      <c r="I16" s="72"/>
+      <c r="J16" s="73"/>
       <c r="K16" s="27"/>
-      <c r="L16" s="67"/>
-      <c r="M16" s="72"/>
-      <c r="N16" s="73"/>
-      <c r="O16" s="74"/>
+      <c r="L16" s="66"/>
+      <c r="M16" s="71"/>
+      <c r="N16" s="72"/>
+      <c r="O16" s="73"/>
       <c r="P16" s="38"/>
       <c r="Q16" s="17"/>
       <c r="R16" s="17"/>
@@ -32795,19 +32913,19 @@
     <row r="17" spans="1:26" ht="19.5" customHeight="1">
       <c r="A17" s="17"/>
       <c r="B17" s="37"/>
-      <c r="C17" s="68"/>
-      <c r="D17" s="75"/>
-      <c r="E17" s="77"/>
+      <c r="C17" s="67"/>
+      <c r="D17" s="74"/>
+      <c r="E17" s="76"/>
       <c r="F17" s="27"/>
-      <c r="G17" s="68"/>
-      <c r="H17" s="75"/>
-      <c r="I17" s="76"/>
-      <c r="J17" s="77"/>
+      <c r="G17" s="67"/>
+      <c r="H17" s="74"/>
+      <c r="I17" s="75"/>
+      <c r="J17" s="76"/>
       <c r="K17" s="27"/>
-      <c r="L17" s="68"/>
-      <c r="M17" s="75"/>
-      <c r="N17" s="76"/>
-      <c r="O17" s="77"/>
+      <c r="L17" s="67"/>
+      <c r="M17" s="74"/>
+      <c r="N17" s="75"/>
+      <c r="O17" s="76"/>
       <c r="P17" s="38"/>
       <c r="Q17" s="17"/>
       <c r="R17" s="17"/>
@@ -32850,42 +32968,42 @@
     </row>
     <row r="19" spans="1:26" ht="19.5" customHeight="1">
       <c r="B19" s="37"/>
-      <c r="C19" s="86" t="s">
-        <v>102</v>
+      <c r="C19" s="85" t="s">
+        <v>98</v>
       </c>
-      <c r="D19" s="71"/>
-      <c r="E19" s="78" t="e">
+      <c r="D19" s="70"/>
+      <c r="E19" s="77" t="str">
         <f>VLOOKUP(C10,'Formato descripción HU'!B6:O23,14,0)</f>
-        <v>#N/A</v>
+        <v xml:space="preserve"> Asignación automática</v>
       </c>
-      <c r="F19" s="79"/>
-      <c r="G19" s="79"/>
-      <c r="H19" s="79"/>
-      <c r="I19" s="79"/>
-      <c r="J19" s="79"/>
-      <c r="K19" s="79"/>
-      <c r="L19" s="79"/>
-      <c r="M19" s="79"/>
-      <c r="N19" s="79"/>
-      <c r="O19" s="80"/>
+      <c r="F19" s="78"/>
+      <c r="G19" s="78"/>
+      <c r="H19" s="78"/>
+      <c r="I19" s="78"/>
+      <c r="J19" s="78"/>
+      <c r="K19" s="78"/>
+      <c r="L19" s="78"/>
+      <c r="M19" s="78"/>
+      <c r="N19" s="78"/>
+      <c r="O19" s="79"/>
       <c r="P19" s="38"/>
       <c r="Q19" s="17"/>
     </row>
     <row r="20" spans="1:26" ht="19.5" customHeight="1">
       <c r="B20" s="37"/>
-      <c r="C20" s="75"/>
-      <c r="D20" s="77"/>
-      <c r="E20" s="81"/>
-      <c r="F20" s="82"/>
-      <c r="G20" s="82"/>
-      <c r="H20" s="82"/>
-      <c r="I20" s="82"/>
-      <c r="J20" s="82"/>
-      <c r="K20" s="82"/>
-      <c r="L20" s="82"/>
-      <c r="M20" s="82"/>
-      <c r="N20" s="82"/>
-      <c r="O20" s="83"/>
+      <c r="C20" s="74"/>
+      <c r="D20" s="76"/>
+      <c r="E20" s="80"/>
+      <c r="F20" s="81"/>
+      <c r="G20" s="81"/>
+      <c r="H20" s="81"/>
+      <c r="I20" s="81"/>
+      <c r="J20" s="81"/>
+      <c r="K20" s="81"/>
+      <c r="L20" s="81"/>
+      <c r="M20" s="81"/>
+      <c r="N20" s="81"/>
+      <c r="O20" s="82"/>
       <c r="P20" s="38"/>
       <c r="Q20" s="17"/>
     </row>
@@ -32910,29 +33028,29 @@
     <row r="22" spans="1:26" ht="19.5" customHeight="1">
       <c r="A22" s="17"/>
       <c r="B22" s="37"/>
-      <c r="C22" s="87" t="s">
-        <v>103</v>
+      <c r="C22" s="86" t="s">
+        <v>99</v>
       </c>
-      <c r="D22" s="71"/>
-      <c r="E22" s="88" t="e">
+      <c r="D22" s="70"/>
+      <c r="E22" s="87" t="str">
         <f>VLOOKUP(C10,'Formato descripción HU'!B6:O23,12,0)</f>
-        <v>#N/A</v>
+        <v>Asignación inmediata y bloqueo en BD al solicitar.</v>
       </c>
-      <c r="F22" s="70"/>
-      <c r="G22" s="70"/>
-      <c r="H22" s="71"/>
+      <c r="F22" s="69"/>
+      <c r="G22" s="69"/>
+      <c r="H22" s="70"/>
       <c r="I22" s="21"/>
-      <c r="J22" s="87" t="s">
+      <c r="J22" s="86" t="s">
         <v>13</v>
       </c>
-      <c r="K22" s="71"/>
-      <c r="L22" s="90" t="e">
+      <c r="K22" s="70"/>
+      <c r="L22" s="89" t="str">
         <f>VLOOKUP(C10,'Formato descripción HU'!B6:O23,13,0)</f>
-        <v>#N/A</v>
+        <v>Riesgo Alto (complejidad lógica).</v>
       </c>
-      <c r="M22" s="70"/>
-      <c r="N22" s="70"/>
-      <c r="O22" s="71"/>
+      <c r="M22" s="69"/>
+      <c r="N22" s="69"/>
+      <c r="O22" s="70"/>
       <c r="P22" s="38"/>
       <c r="Q22" s="17"/>
       <c r="R22" s="17"/>
@@ -32948,19 +33066,19 @@
     <row r="23" spans="1:26" ht="19.5" customHeight="1">
       <c r="A23" s="17"/>
       <c r="B23" s="37"/>
-      <c r="C23" s="72"/>
-      <c r="D23" s="74"/>
-      <c r="E23" s="72"/>
-      <c r="F23" s="73"/>
-      <c r="G23" s="73"/>
-      <c r="H23" s="74"/>
+      <c r="C23" s="71"/>
+      <c r="D23" s="73"/>
+      <c r="E23" s="71"/>
+      <c r="F23" s="72"/>
+      <c r="G23" s="72"/>
+      <c r="H23" s="73"/>
       <c r="I23" s="21"/>
-      <c r="J23" s="72"/>
-      <c r="K23" s="74"/>
-      <c r="L23" s="72"/>
-      <c r="M23" s="73"/>
-      <c r="N23" s="73"/>
-      <c r="O23" s="74"/>
+      <c r="J23" s="71"/>
+      <c r="K23" s="73"/>
+      <c r="L23" s="71"/>
+      <c r="M23" s="72"/>
+      <c r="N23" s="72"/>
+      <c r="O23" s="73"/>
       <c r="P23" s="38"/>
       <c r="Q23" s="17"/>
       <c r="R23" s="17"/>
@@ -32976,19 +33094,2183 @@
     <row r="24" spans="1:26" ht="19.5" customHeight="1">
       <c r="A24" s="17"/>
       <c r="B24" s="37"/>
-      <c r="C24" s="75"/>
-      <c r="D24" s="77"/>
-      <c r="E24" s="75"/>
-      <c r="F24" s="76"/>
-      <c r="G24" s="76"/>
-      <c r="H24" s="77"/>
+      <c r="C24" s="74"/>
+      <c r="D24" s="76"/>
+      <c r="E24" s="74"/>
+      <c r="F24" s="75"/>
+      <c r="G24" s="75"/>
+      <c r="H24" s="76"/>
       <c r="I24" s="21"/>
-      <c r="J24" s="75"/>
-      <c r="K24" s="77"/>
-      <c r="L24" s="75"/>
-      <c r="M24" s="76"/>
-      <c r="N24" s="76"/>
-      <c r="O24" s="77"/>
+      <c r="J24" s="74"/>
+      <c r="K24" s="76"/>
+      <c r="L24" s="74"/>
+      <c r="M24" s="75"/>
+      <c r="N24" s="75"/>
+      <c r="O24" s="76"/>
+      <c r="P24" s="38"/>
+      <c r="Q24" s="17"/>
+      <c r="R24" s="17"/>
+      <c r="S24" s="17"/>
+      <c r="T24" s="17"/>
+      <c r="U24" s="17"/>
+      <c r="V24" s="17"/>
+      <c r="W24" s="17"/>
+      <c r="X24" s="17"/>
+      <c r="Y24" s="17"/>
+      <c r="Z24" s="17"/>
+    </row>
+    <row r="25" spans="1:26" ht="9.75" customHeight="1">
+      <c r="A25" s="17"/>
+      <c r="B25" s="28"/>
+      <c r="C25" s="29"/>
+      <c r="D25" s="29"/>
+      <c r="E25" s="29"/>
+      <c r="F25" s="29"/>
+      <c r="G25" s="29"/>
+      <c r="H25" s="29"/>
+      <c r="I25" s="29"/>
+      <c r="J25" s="29"/>
+      <c r="K25" s="29"/>
+      <c r="L25" s="29"/>
+      <c r="M25" s="29"/>
+      <c r="N25" s="29"/>
+      <c r="O25" s="29"/>
+      <c r="P25" s="30"/>
+      <c r="Q25" s="17"/>
+      <c r="R25" s="17"/>
+      <c r="S25" s="17"/>
+      <c r="T25" s="17"/>
+      <c r="U25" s="17"/>
+      <c r="V25" s="17"/>
+      <c r="W25" s="17"/>
+      <c r="X25" s="17"/>
+      <c r="Y25" s="17"/>
+      <c r="Z25" s="17"/>
+    </row>
+    <row r="26" spans="1:26" ht="19.5" customHeight="1">
+      <c r="A26" s="17"/>
+      <c r="B26" s="17"/>
+      <c r="C26" s="17"/>
+      <c r="D26" s="17"/>
+      <c r="E26" s="17"/>
+      <c r="F26" s="17"/>
+      <c r="G26" s="17"/>
+      <c r="H26" s="17"/>
+      <c r="I26" s="17"/>
+      <c r="J26" s="17"/>
+      <c r="K26" s="17"/>
+      <c r="L26" s="17"/>
+      <c r="M26" s="17"/>
+      <c r="N26" s="17"/>
+      <c r="O26" s="17"/>
+      <c r="P26" s="17"/>
+      <c r="Q26" s="17"/>
+      <c r="R26" s="17"/>
+      <c r="S26" s="17"/>
+      <c r="T26" s="17"/>
+      <c r="U26" s="17"/>
+      <c r="V26" s="17"/>
+      <c r="W26" s="17"/>
+      <c r="X26" s="17"/>
+      <c r="Y26" s="17"/>
+      <c r="Z26" s="17"/>
+    </row>
+    <row r="27" spans="1:26" ht="19.5" customHeight="1">
+      <c r="A27" s="17"/>
+      <c r="B27" s="17"/>
+      <c r="C27" s="17"/>
+      <c r="D27" s="17"/>
+      <c r="E27" s="17"/>
+      <c r="F27" s="17"/>
+      <c r="G27" s="17"/>
+      <c r="H27" s="17"/>
+      <c r="I27" s="17"/>
+      <c r="J27" s="17"/>
+      <c r="K27" s="17"/>
+      <c r="L27" s="17"/>
+      <c r="M27" s="17"/>
+      <c r="N27" s="17"/>
+      <c r="O27" s="17"/>
+      <c r="P27" s="17"/>
+      <c r="Q27" s="17"/>
+      <c r="R27" s="17"/>
+      <c r="S27" s="17"/>
+      <c r="T27" s="17"/>
+      <c r="U27" s="17"/>
+      <c r="V27" s="17"/>
+      <c r="W27" s="17"/>
+      <c r="X27" s="17"/>
+      <c r="Y27" s="17"/>
+      <c r="Z27" s="17"/>
+    </row>
+    <row r="28" spans="1:26" ht="19.5" customHeight="1">
+      <c r="A28" s="17"/>
+      <c r="B28" s="17"/>
+      <c r="C28" s="17"/>
+      <c r="D28" s="17"/>
+      <c r="E28" s="17"/>
+      <c r="F28" s="17"/>
+      <c r="G28" s="17"/>
+      <c r="H28" s="17"/>
+      <c r="I28" s="17"/>
+      <c r="J28" s="17"/>
+      <c r="K28" s="17"/>
+      <c r="L28" s="17"/>
+      <c r="M28" s="17"/>
+      <c r="N28" s="17"/>
+      <c r="O28" s="17"/>
+      <c r="P28" s="17"/>
+      <c r="Q28" s="17"/>
+      <c r="R28" s="17"/>
+      <c r="S28" s="17"/>
+      <c r="T28" s="17"/>
+      <c r="U28" s="17"/>
+      <c r="V28" s="17"/>
+      <c r="W28" s="17"/>
+      <c r="X28" s="17"/>
+      <c r="Y28" s="17"/>
+      <c r="Z28" s="17"/>
+    </row>
+    <row r="29" spans="1:26" ht="19.5" customHeight="1">
+      <c r="A29" s="17"/>
+      <c r="B29" s="17"/>
+      <c r="C29" s="17"/>
+      <c r="D29" s="17"/>
+      <c r="E29" s="17"/>
+      <c r="F29" s="17"/>
+      <c r="G29" s="17"/>
+      <c r="H29" s="17"/>
+      <c r="I29" s="17"/>
+      <c r="J29" s="17"/>
+      <c r="K29" s="17"/>
+      <c r="L29" s="17"/>
+      <c r="M29" s="17"/>
+      <c r="N29" s="17"/>
+      <c r="O29" s="17"/>
+      <c r="P29" s="17"/>
+      <c r="Q29" s="17"/>
+      <c r="R29" s="17"/>
+      <c r="S29" s="17"/>
+      <c r="T29" s="17"/>
+      <c r="U29" s="17"/>
+      <c r="V29" s="17"/>
+      <c r="W29" s="17"/>
+      <c r="X29" s="17"/>
+      <c r="Y29" s="17"/>
+      <c r="Z29" s="17"/>
+    </row>
+    <row r="30" spans="1:26" ht="19.5" customHeight="1">
+      <c r="A30" s="17"/>
+      <c r="B30" s="17"/>
+      <c r="C30" s="17"/>
+      <c r="D30" s="17"/>
+      <c r="E30" s="17"/>
+      <c r="F30" s="17"/>
+      <c r="G30" s="17"/>
+      <c r="H30" s="17"/>
+      <c r="I30" s="17"/>
+      <c r="J30" s="17"/>
+      <c r="K30" s="17"/>
+      <c r="L30" s="17"/>
+      <c r="M30" s="17"/>
+      <c r="N30" s="17"/>
+      <c r="O30" s="17"/>
+      <c r="P30" s="17"/>
+      <c r="Q30" s="17"/>
+      <c r="R30" s="17"/>
+      <c r="S30" s="17"/>
+      <c r="T30" s="17"/>
+      <c r="U30" s="17"/>
+      <c r="V30" s="17"/>
+      <c r="W30" s="17"/>
+      <c r="X30" s="17"/>
+      <c r="Y30" s="17"/>
+      <c r="Z30" s="17"/>
+    </row>
+    <row r="31" spans="1:26" ht="19.5" customHeight="1">
+      <c r="A31" s="17"/>
+      <c r="B31" s="17"/>
+      <c r="C31" s="17"/>
+      <c r="D31" s="17"/>
+      <c r="E31" s="17"/>
+      <c r="F31" s="17"/>
+      <c r="G31" s="17"/>
+      <c r="H31" s="17"/>
+      <c r="I31" s="17"/>
+      <c r="J31" s="17"/>
+      <c r="K31" s="17"/>
+      <c r="L31" s="17"/>
+      <c r="M31" s="17"/>
+      <c r="N31" s="17"/>
+      <c r="O31" s="17"/>
+      <c r="P31" s="17"/>
+      <c r="Q31" s="17"/>
+      <c r="R31" s="17"/>
+      <c r="S31" s="17"/>
+      <c r="T31" s="17"/>
+      <c r="U31" s="17"/>
+      <c r="V31" s="17"/>
+      <c r="W31" s="17"/>
+      <c r="X31" s="17"/>
+      <c r="Y31" s="17"/>
+      <c r="Z31" s="17"/>
+    </row>
+    <row r="32" spans="1:26" ht="19.5" customHeight="1">
+      <c r="A32" s="17"/>
+      <c r="B32" s="17"/>
+      <c r="C32" s="17"/>
+      <c r="D32" s="17"/>
+      <c r="E32" s="17"/>
+      <c r="F32" s="17"/>
+      <c r="G32" s="17"/>
+      <c r="H32" s="17"/>
+      <c r="I32" s="17"/>
+      <c r="J32" s="17"/>
+      <c r="K32" s="17"/>
+      <c r="L32" s="17"/>
+      <c r="M32" s="17"/>
+      <c r="N32" s="17"/>
+      <c r="O32" s="17"/>
+      <c r="P32" s="17"/>
+      <c r="Q32" s="17"/>
+      <c r="R32" s="17"/>
+      <c r="S32" s="17"/>
+      <c r="T32" s="17"/>
+      <c r="U32" s="17"/>
+      <c r="V32" s="17"/>
+      <c r="W32" s="17"/>
+      <c r="X32" s="17"/>
+      <c r="Y32" s="17"/>
+      <c r="Z32" s="17"/>
+    </row>
+    <row r="33" spans="1:26" ht="19.5" customHeight="1">
+      <c r="A33" s="17"/>
+      <c r="B33" s="17"/>
+      <c r="C33" s="17"/>
+      <c r="D33" s="17"/>
+      <c r="E33" s="17"/>
+      <c r="F33" s="17"/>
+      <c r="G33" s="17"/>
+      <c r="H33" s="17"/>
+      <c r="I33" s="17"/>
+      <c r="J33" s="17"/>
+      <c r="K33" s="17"/>
+      <c r="L33" s="17"/>
+      <c r="M33" s="17"/>
+      <c r="N33" s="17"/>
+      <c r="O33" s="17"/>
+      <c r="P33" s="17"/>
+      <c r="Q33" s="17"/>
+      <c r="R33" s="17"/>
+      <c r="S33" s="17"/>
+      <c r="T33" s="17"/>
+      <c r="U33" s="17"/>
+      <c r="V33" s="17"/>
+      <c r="W33" s="17"/>
+      <c r="X33" s="17"/>
+      <c r="Y33" s="17"/>
+      <c r="Z33" s="17"/>
+    </row>
+    <row r="34" spans="1:26" ht="19.5" customHeight="1">
+      <c r="C34" s="17"/>
+      <c r="D34" s="17"/>
+      <c r="E34" s="17"/>
+      <c r="F34" s="17"/>
+      <c r="G34" s="17"/>
+      <c r="H34" s="17"/>
+      <c r="I34" s="17"/>
+      <c r="J34" s="17"/>
+      <c r="K34" s="17"/>
+      <c r="L34" s="17"/>
+      <c r="M34" s="17"/>
+      <c r="N34" s="17"/>
+      <c r="O34" s="17"/>
+      <c r="P34" s="17"/>
+    </row>
+    <row r="35" spans="1:26" ht="19.5" customHeight="1">
+      <c r="C35" s="17"/>
+      <c r="D35" s="17"/>
+      <c r="E35" s="17"/>
+      <c r="F35" s="17"/>
+      <c r="G35" s="17"/>
+      <c r="H35" s="17"/>
+      <c r="I35" s="17"/>
+      <c r="J35" s="17"/>
+      <c r="K35" s="17"/>
+      <c r="L35" s="17"/>
+      <c r="M35" s="17"/>
+      <c r="N35" s="17"/>
+      <c r="O35" s="17"/>
+      <c r="P35" s="17"/>
+    </row>
+    <row r="36" spans="1:26" ht="19.5" customHeight="1">
+      <c r="C36" s="17"/>
+      <c r="D36" s="17"/>
+      <c r="E36" s="17"/>
+      <c r="F36" s="17"/>
+      <c r="G36" s="17"/>
+      <c r="H36" s="17"/>
+      <c r="I36" s="17"/>
+      <c r="J36" s="17"/>
+      <c r="K36" s="17"/>
+      <c r="L36" s="17"/>
+      <c r="M36" s="17"/>
+      <c r="N36" s="17"/>
+      <c r="O36" s="17"/>
+      <c r="P36" s="17"/>
+    </row>
+    <row r="37" spans="1:26" ht="19.5" customHeight="1">
+      <c r="C37" s="17"/>
+      <c r="D37" s="17"/>
+      <c r="E37" s="17"/>
+      <c r="F37" s="17"/>
+      <c r="G37" s="17"/>
+      <c r="H37" s="17"/>
+      <c r="I37" s="17"/>
+      <c r="J37" s="17"/>
+      <c r="K37" s="17"/>
+      <c r="L37" s="17"/>
+      <c r="M37" s="17"/>
+      <c r="N37" s="17"/>
+      <c r="O37" s="17"/>
+      <c r="P37" s="17"/>
+    </row>
+    <row r="38" spans="1:26" ht="19.5" customHeight="1">
+      <c r="C38" s="17"/>
+      <c r="D38" s="17"/>
+      <c r="E38" s="17"/>
+      <c r="F38" s="17"/>
+      <c r="G38" s="17"/>
+      <c r="H38" s="17"/>
+      <c r="I38" s="17"/>
+      <c r="J38" s="17"/>
+      <c r="K38" s="17"/>
+      <c r="L38" s="17"/>
+      <c r="M38" s="17"/>
+      <c r="N38" s="17"/>
+      <c r="O38" s="17"/>
+      <c r="P38" s="17"/>
+    </row>
+    <row r="39" spans="1:26" ht="19.5" customHeight="1">
+      <c r="C39" s="17"/>
+      <c r="D39" s="17"/>
+      <c r="E39" s="17"/>
+      <c r="F39" s="17"/>
+      <c r="G39" s="17"/>
+      <c r="H39" s="17"/>
+      <c r="I39" s="17"/>
+      <c r="J39" s="17"/>
+      <c r="K39" s="17"/>
+      <c r="L39" s="17"/>
+      <c r="M39" s="17"/>
+      <c r="N39" s="17"/>
+      <c r="O39" s="17"/>
+      <c r="P39" s="17"/>
+    </row>
+    <row r="40" spans="1:26" ht="19.5" customHeight="1">
+      <c r="F40" s="17"/>
+      <c r="G40" s="17"/>
+      <c r="H40" s="17"/>
+      <c r="I40" s="17"/>
+      <c r="J40" s="17"/>
+      <c r="K40" s="17"/>
+      <c r="L40" s="17"/>
+      <c r="M40" s="17"/>
+      <c r="N40" s="17"/>
+      <c r="O40" s="17"/>
+      <c r="P40" s="17"/>
+    </row>
+    <row r="41" spans="1:26" ht="19.5" customHeight="1">
+      <c r="C41" s="17"/>
+      <c r="D41" s="17"/>
+      <c r="E41" s="17"/>
+      <c r="F41" s="17"/>
+      <c r="G41" s="17"/>
+      <c r="H41" s="17"/>
+      <c r="I41" s="17"/>
+      <c r="J41" s="17"/>
+      <c r="K41" s="17"/>
+      <c r="L41" s="17"/>
+      <c r="M41" s="17"/>
+      <c r="N41" s="17"/>
+      <c r="O41" s="17"/>
+      <c r="P41" s="17"/>
+    </row>
+    <row r="42" spans="1:26" ht="19.5" customHeight="1">
+      <c r="C42" s="17"/>
+      <c r="D42" s="17"/>
+      <c r="E42" s="17"/>
+      <c r="F42" s="17"/>
+      <c r="G42" s="17"/>
+      <c r="H42" s="17"/>
+      <c r="I42" s="17"/>
+      <c r="J42" s="17"/>
+      <c r="K42" s="17"/>
+      <c r="L42" s="17"/>
+      <c r="M42" s="17"/>
+      <c r="N42" s="17"/>
+      <c r="O42" s="17"/>
+      <c r="P42" s="17"/>
+    </row>
+    <row r="43" spans="1:26" ht="19.5" customHeight="1">
+      <c r="C43" s="17"/>
+      <c r="D43" s="17"/>
+      <c r="E43" s="17"/>
+      <c r="F43" s="17"/>
+      <c r="G43" s="17"/>
+      <c r="H43" s="17"/>
+      <c r="I43" s="17"/>
+      <c r="J43" s="17"/>
+      <c r="K43" s="17"/>
+      <c r="L43" s="17"/>
+      <c r="M43" s="17"/>
+      <c r="N43" s="17"/>
+      <c r="O43" s="17"/>
+      <c r="P43" s="17"/>
+    </row>
+    <row r="44" spans="1:26" ht="19.5" customHeight="1">
+      <c r="C44" s="17"/>
+      <c r="D44" s="17"/>
+      <c r="E44" s="17"/>
+      <c r="F44" s="17"/>
+      <c r="G44" s="17"/>
+      <c r="H44" s="17"/>
+      <c r="I44" s="17"/>
+      <c r="J44" s="17"/>
+      <c r="K44" s="17"/>
+      <c r="L44" s="17"/>
+      <c r="M44" s="17"/>
+      <c r="N44" s="17"/>
+      <c r="O44" s="17"/>
+      <c r="P44" s="17"/>
+    </row>
+    <row r="45" spans="1:26" ht="19.5" customHeight="1">
+      <c r="C45" s="17"/>
+      <c r="D45" s="17"/>
+      <c r="E45" s="17"/>
+      <c r="F45" s="17"/>
+      <c r="G45" s="17"/>
+      <c r="H45" s="17"/>
+      <c r="I45" s="17"/>
+      <c r="J45" s="17"/>
+      <c r="K45" s="17"/>
+      <c r="L45" s="17"/>
+      <c r="M45" s="17"/>
+      <c r="N45" s="17"/>
+      <c r="O45" s="17"/>
+      <c r="P45" s="17"/>
+    </row>
+    <row r="46" spans="1:26" ht="19.5" customHeight="1">
+      <c r="C46" s="17"/>
+      <c r="D46" s="17"/>
+      <c r="E46" s="17"/>
+      <c r="F46" s="17"/>
+      <c r="G46" s="17"/>
+      <c r="H46" s="17"/>
+      <c r="I46" s="17"/>
+      <c r="J46" s="17"/>
+      <c r="K46" s="17"/>
+      <c r="L46" s="17"/>
+      <c r="M46" s="17"/>
+      <c r="N46" s="17"/>
+      <c r="O46" s="17"/>
+      <c r="P46" s="17"/>
+    </row>
+    <row r="47" spans="1:26" ht="19.5" customHeight="1">
+      <c r="C47" s="17"/>
+      <c r="D47" s="17"/>
+      <c r="E47" s="17"/>
+      <c r="F47" s="17"/>
+      <c r="G47" s="17"/>
+      <c r="H47" s="17"/>
+      <c r="I47" s="17"/>
+      <c r="J47" s="17"/>
+      <c r="K47" s="17"/>
+      <c r="L47" s="17"/>
+      <c r="M47" s="17"/>
+      <c r="N47" s="17"/>
+      <c r="O47" s="17"/>
+      <c r="P47" s="17"/>
+    </row>
+    <row r="48" spans="1:26" ht="19.5" customHeight="1">
+      <c r="C48" s="17"/>
+      <c r="D48" s="17"/>
+      <c r="E48" s="17"/>
+      <c r="F48" s="17"/>
+      <c r="G48" s="17"/>
+      <c r="H48" s="17"/>
+      <c r="I48" s="17"/>
+      <c r="J48" s="17"/>
+      <c r="K48" s="17"/>
+      <c r="L48" s="17"/>
+      <c r="M48" s="17"/>
+      <c r="N48" s="17"/>
+      <c r="O48" s="17"/>
+      <c r="P48" s="17"/>
+    </row>
+    <row r="49" spans="3:16" ht="19.5" customHeight="1">
+      <c r="C49" s="17"/>
+      <c r="D49" s="17"/>
+      <c r="E49" s="17"/>
+      <c r="F49" s="17"/>
+      <c r="G49" s="17"/>
+      <c r="H49" s="17"/>
+      <c r="I49" s="17"/>
+      <c r="J49" s="17"/>
+      <c r="K49" s="17"/>
+      <c r="L49" s="17"/>
+      <c r="M49" s="17"/>
+      <c r="N49" s="17"/>
+      <c r="O49" s="17"/>
+      <c r="P49" s="17"/>
+    </row>
+    <row r="50" spans="3:16" ht="19.5" customHeight="1">
+      <c r="C50" s="17"/>
+      <c r="D50" s="17"/>
+      <c r="E50" s="17"/>
+      <c r="F50" s="17"/>
+      <c r="G50" s="17"/>
+      <c r="H50" s="17"/>
+      <c r="I50" s="17"/>
+      <c r="J50" s="17"/>
+      <c r="K50" s="17"/>
+      <c r="L50" s="17"/>
+      <c r="M50" s="17"/>
+      <c r="N50" s="17"/>
+      <c r="O50" s="17"/>
+      <c r="P50" s="17"/>
+    </row>
+    <row r="51" spans="3:16" ht="19.5" customHeight="1">
+      <c r="C51" s="17"/>
+      <c r="D51" s="17"/>
+      <c r="E51" s="17"/>
+      <c r="F51" s="17"/>
+      <c r="G51" s="17"/>
+      <c r="H51" s="17"/>
+      <c r="I51" s="17"/>
+      <c r="J51" s="17"/>
+      <c r="K51" s="17"/>
+      <c r="L51" s="17"/>
+      <c r="M51" s="17"/>
+      <c r="N51" s="17"/>
+      <c r="O51" s="17"/>
+      <c r="P51" s="17"/>
+    </row>
+    <row r="52" spans="3:16" ht="19.5" customHeight="1">
+      <c r="C52" s="17"/>
+      <c r="D52" s="17"/>
+      <c r="E52" s="17"/>
+      <c r="F52" s="17"/>
+      <c r="G52" s="17"/>
+      <c r="H52" s="17"/>
+      <c r="I52" s="17"/>
+      <c r="J52" s="17"/>
+      <c r="K52" s="17"/>
+      <c r="L52" s="17"/>
+      <c r="M52" s="17"/>
+      <c r="N52" s="17"/>
+      <c r="O52" s="17"/>
+      <c r="P52" s="17"/>
+    </row>
+    <row r="53" spans="3:16" ht="19.5" customHeight="1">
+      <c r="C53" s="17"/>
+      <c r="D53" s="17"/>
+      <c r="E53" s="17"/>
+      <c r="F53" s="17"/>
+      <c r="G53" s="17"/>
+      <c r="H53" s="17"/>
+      <c r="I53" s="17"/>
+      <c r="J53" s="17"/>
+      <c r="K53" s="17"/>
+      <c r="L53" s="17"/>
+      <c r="M53" s="17"/>
+      <c r="N53" s="17"/>
+      <c r="O53" s="17"/>
+      <c r="P53" s="17"/>
+    </row>
+    <row r="54" spans="3:16" ht="19.5" customHeight="1">
+      <c r="C54" s="17"/>
+      <c r="D54" s="17"/>
+      <c r="E54" s="17"/>
+      <c r="F54" s="17"/>
+      <c r="G54" s="17"/>
+      <c r="H54" s="17"/>
+      <c r="I54" s="17"/>
+      <c r="J54" s="17"/>
+      <c r="K54" s="17"/>
+      <c r="L54" s="17"/>
+      <c r="M54" s="17"/>
+      <c r="N54" s="17"/>
+      <c r="O54" s="17"/>
+    </row>
+    <row r="55" spans="3:16" ht="15.75" customHeight="1">
+      <c r="C55" s="17"/>
+      <c r="D55" s="17"/>
+      <c r="E55" s="17"/>
+      <c r="F55" s="17"/>
+      <c r="G55" s="17"/>
+      <c r="H55" s="17"/>
+      <c r="I55" s="17"/>
+      <c r="J55" s="17"/>
+      <c r="K55" s="17"/>
+      <c r="L55" s="17"/>
+      <c r="M55" s="17"/>
+      <c r="N55" s="17"/>
+      <c r="O55" s="17"/>
+    </row>
+    <row r="56" spans="3:16" ht="15.75" customHeight="1"/>
+    <row r="57" spans="3:16" ht="15.75" customHeight="1"/>
+    <row r="58" spans="3:16" ht="15.75" customHeight="1"/>
+    <row r="59" spans="3:16" ht="15.75" customHeight="1"/>
+    <row r="60" spans="3:16" ht="15.75" customHeight="1"/>
+    <row r="61" spans="3:16" ht="15.75" customHeight="1"/>
+    <row r="62" spans="3:16" ht="15.75" customHeight="1"/>
+    <row r="63" spans="3:16" ht="15.75" customHeight="1"/>
+    <row r="64" spans="3:16" ht="15.75" customHeight="1"/>
+    <row r="65" ht="15.75" customHeight="1"/>
+    <row r="66" ht="15.75" customHeight="1"/>
+    <row r="67" ht="15.75" customHeight="1"/>
+    <row r="68" ht="15.75" customHeight="1"/>
+    <row r="69" ht="15.75" customHeight="1"/>
+    <row r="70" ht="15.75" customHeight="1"/>
+    <row r="71" ht="15.75" customHeight="1"/>
+    <row r="72" ht="15.75" customHeight="1"/>
+    <row r="73" ht="15.75" customHeight="1"/>
+    <row r="74" ht="15.75" customHeight="1"/>
+    <row r="75" ht="15.75" customHeight="1"/>
+    <row r="76" ht="15.75" customHeight="1"/>
+    <row r="77" ht="15.75" customHeight="1"/>
+    <row r="78" ht="15.75" customHeight="1"/>
+    <row r="79" ht="15.75" customHeight="1"/>
+    <row r="80" ht="15.75" customHeight="1"/>
+    <row r="81" ht="15.75" customHeight="1"/>
+    <row r="82" ht="15.75" customHeight="1"/>
+    <row r="83" ht="15.75" customHeight="1"/>
+    <row r="84" ht="15.75" customHeight="1"/>
+    <row r="85" ht="15.75" customHeight="1"/>
+    <row r="86" ht="15.75" customHeight="1"/>
+    <row r="87" ht="15.75" customHeight="1"/>
+    <row r="88" ht="15.75" customHeight="1"/>
+    <row r="89" ht="15.75" customHeight="1"/>
+    <row r="90" ht="15.75" customHeight="1"/>
+    <row r="91" ht="15.75" customHeight="1"/>
+    <row r="92" ht="15.75" customHeight="1"/>
+    <row r="93" ht="15.75" customHeight="1"/>
+    <row r="94" ht="15.75" customHeight="1"/>
+    <row r="95" ht="15.75" customHeight="1"/>
+    <row r="96" ht="15.75" customHeight="1"/>
+    <row r="97" ht="15.75" customHeight="1"/>
+    <row r="98" ht="15.75" customHeight="1"/>
+    <row r="99" ht="15.75" customHeight="1"/>
+    <row r="100" ht="15.75" customHeight="1"/>
+    <row r="101" ht="15.75" customHeight="1"/>
+    <row r="102" ht="15.75" customHeight="1"/>
+    <row r="103" ht="15.75" customHeight="1"/>
+    <row r="104" ht="15.75" customHeight="1"/>
+    <row r="105" ht="15.75" customHeight="1"/>
+    <row r="106" ht="15.75" customHeight="1"/>
+    <row r="107" ht="15.75" customHeight="1"/>
+    <row r="108" ht="15.75" customHeight="1"/>
+    <row r="109" ht="15.75" customHeight="1"/>
+    <row r="110" ht="15.75" customHeight="1"/>
+    <row r="111" ht="15.75" customHeight="1"/>
+    <row r="112" ht="15.75" customHeight="1"/>
+    <row r="113" ht="15.75" customHeight="1"/>
+    <row r="114" ht="15.75" customHeight="1"/>
+    <row r="115" ht="15.75" customHeight="1"/>
+    <row r="116" ht="15.75" customHeight="1"/>
+    <row r="117" ht="15.75" customHeight="1"/>
+    <row r="118" ht="15.75" customHeight="1"/>
+    <row r="119" ht="15.75" customHeight="1"/>
+    <row r="120" ht="15.75" customHeight="1"/>
+    <row r="121" ht="15.75" customHeight="1"/>
+    <row r="122" ht="15.75" customHeight="1"/>
+    <row r="123" ht="15.75" customHeight="1"/>
+    <row r="124" ht="15.75" customHeight="1"/>
+    <row r="125" ht="15.75" customHeight="1"/>
+    <row r="126" ht="15.75" customHeight="1"/>
+    <row r="127" ht="15.75" customHeight="1"/>
+    <row r="128" ht="15.75" customHeight="1"/>
+    <row r="129" ht="15.75" customHeight="1"/>
+    <row r="130" ht="15.75" customHeight="1"/>
+    <row r="131" ht="15.75" customHeight="1"/>
+    <row r="132" ht="15.75" customHeight="1"/>
+    <row r="133" ht="15.75" customHeight="1"/>
+    <row r="134" ht="15.75" customHeight="1"/>
+    <row r="135" ht="15.75" customHeight="1"/>
+    <row r="136" ht="15.75" customHeight="1"/>
+    <row r="137" ht="15.75" customHeight="1"/>
+    <row r="138" ht="15.75" customHeight="1"/>
+    <row r="139" ht="15.75" customHeight="1"/>
+    <row r="140" ht="15.75" customHeight="1"/>
+    <row r="141" ht="15.75" customHeight="1"/>
+    <row r="142" ht="15.75" customHeight="1"/>
+    <row r="143" ht="15.75" customHeight="1"/>
+    <row r="144" ht="15.75" customHeight="1"/>
+    <row r="145" ht="15.75" customHeight="1"/>
+    <row r="146" ht="15.75" customHeight="1"/>
+    <row r="147" ht="15.75" customHeight="1"/>
+    <row r="148" ht="15.75" customHeight="1"/>
+    <row r="149" ht="15.75" customHeight="1"/>
+    <row r="150" ht="15.75" customHeight="1"/>
+    <row r="151" ht="15.75" customHeight="1"/>
+    <row r="152" ht="15.75" customHeight="1"/>
+    <row r="153" ht="15.75" customHeight="1"/>
+    <row r="154" ht="15.75" customHeight="1"/>
+    <row r="155" ht="15.75" customHeight="1"/>
+    <row r="156" ht="15.75" customHeight="1"/>
+    <row r="157" ht="15.75" customHeight="1"/>
+    <row r="158" ht="15.75" customHeight="1"/>
+    <row r="159" ht="15.75" customHeight="1"/>
+    <row r="160" ht="15.75" customHeight="1"/>
+    <row r="161" ht="15.75" customHeight="1"/>
+    <row r="162" ht="15.75" customHeight="1"/>
+    <row r="163" ht="15.75" customHeight="1"/>
+    <row r="164" ht="15.75" customHeight="1"/>
+    <row r="165" ht="15.75" customHeight="1"/>
+    <row r="166" ht="15.75" customHeight="1"/>
+    <row r="167" ht="15.75" customHeight="1"/>
+    <row r="168" ht="15.75" customHeight="1"/>
+    <row r="169" ht="15.75" customHeight="1"/>
+    <row r="170" ht="15.75" customHeight="1"/>
+    <row r="171" ht="15.75" customHeight="1"/>
+    <row r="172" ht="15.75" customHeight="1"/>
+    <row r="173" ht="15.75" customHeight="1"/>
+    <row r="174" ht="15.75" customHeight="1"/>
+    <row r="175" ht="15.75" customHeight="1"/>
+    <row r="176" ht="15.75" customHeight="1"/>
+    <row r="177" ht="15.75" customHeight="1"/>
+    <row r="178" ht="15.75" customHeight="1"/>
+    <row r="179" ht="15.75" customHeight="1"/>
+    <row r="180" ht="15.75" customHeight="1"/>
+    <row r="181" ht="15.75" customHeight="1"/>
+    <row r="182" ht="15.75" customHeight="1"/>
+    <row r="183" ht="15.75" customHeight="1"/>
+    <row r="184" ht="15.75" customHeight="1"/>
+    <row r="185" ht="15.75" customHeight="1"/>
+    <row r="186" ht="15.75" customHeight="1"/>
+    <row r="187" ht="15.75" customHeight="1"/>
+    <row r="188" ht="15.75" customHeight="1"/>
+    <row r="189" ht="15.75" customHeight="1"/>
+    <row r="190" ht="15.75" customHeight="1"/>
+    <row r="191" ht="15.75" customHeight="1"/>
+    <row r="192" ht="15.75" customHeight="1"/>
+    <row r="193" ht="15.75" customHeight="1"/>
+    <row r="194" ht="15.75" customHeight="1"/>
+    <row r="195" ht="15.75" customHeight="1"/>
+    <row r="196" ht="15.75" customHeight="1"/>
+    <row r="197" ht="15.75" customHeight="1"/>
+    <row r="198" ht="15.75" customHeight="1"/>
+    <row r="199" ht="15.75" customHeight="1"/>
+    <row r="200" ht="15.75" customHeight="1"/>
+    <row r="201" ht="15.75" customHeight="1"/>
+    <row r="202" ht="15.75" customHeight="1"/>
+    <row r="203" ht="15.75" customHeight="1"/>
+    <row r="204" ht="15.75" customHeight="1"/>
+    <row r="205" ht="15.75" customHeight="1"/>
+    <row r="206" ht="15.75" customHeight="1"/>
+    <row r="207" ht="15.75" customHeight="1"/>
+    <row r="208" ht="15.75" customHeight="1"/>
+    <row r="209" ht="15.75" customHeight="1"/>
+    <row r="210" ht="15.75" customHeight="1"/>
+    <row r="211" ht="15.75" customHeight="1"/>
+    <row r="212" ht="15.75" customHeight="1"/>
+    <row r="213" ht="15.75" customHeight="1"/>
+    <row r="214" ht="15.75" customHeight="1"/>
+    <row r="215" ht="15.75" customHeight="1"/>
+    <row r="216" ht="15.75" customHeight="1"/>
+    <row r="217" ht="15.75" customHeight="1"/>
+    <row r="218" ht="15.75" customHeight="1"/>
+    <row r="219" ht="15.75" customHeight="1"/>
+    <row r="220" ht="15.75" customHeight="1"/>
+    <row r="221" ht="15.75" customHeight="1"/>
+    <row r="222" ht="15.75" customHeight="1"/>
+    <row r="223" ht="15.75" customHeight="1"/>
+    <row r="224" ht="15.75" customHeight="1"/>
+    <row r="225" ht="15.75" customHeight="1"/>
+    <row r="226" ht="15.75" customHeight="1"/>
+    <row r="227" ht="15.75" customHeight="1"/>
+    <row r="228" ht="15.75" customHeight="1"/>
+    <row r="229" ht="15.75" customHeight="1"/>
+    <row r="230" ht="15.75" customHeight="1"/>
+    <row r="231" ht="15.75" customHeight="1"/>
+    <row r="232" ht="15.75" customHeight="1"/>
+    <row r="233" ht="15.75" customHeight="1"/>
+    <row r="234" ht="15.75" customHeight="1"/>
+    <row r="235" ht="15.75" customHeight="1"/>
+    <row r="236" ht="15.75" customHeight="1"/>
+    <row r="237" ht="15.75" customHeight="1"/>
+    <row r="238" ht="15.75" customHeight="1"/>
+    <row r="239" ht="15.75" customHeight="1"/>
+    <row r="240" ht="15.75" customHeight="1"/>
+    <row r="241" ht="15.75" customHeight="1"/>
+    <row r="242" ht="15.75" customHeight="1"/>
+    <row r="243" ht="15.75" customHeight="1"/>
+    <row r="244" ht="15.75" customHeight="1"/>
+    <row r="245" ht="15.75" customHeight="1"/>
+    <row r="246" ht="15.75" customHeight="1"/>
+    <row r="247" ht="15.75" customHeight="1"/>
+    <row r="248" ht="15.75" customHeight="1"/>
+    <row r="249" ht="15.75" customHeight="1"/>
+    <row r="250" ht="15.75" customHeight="1"/>
+    <row r="251" ht="15.75" customHeight="1"/>
+    <row r="252" ht="15.75" customHeight="1"/>
+    <row r="253" ht="15.75" customHeight="1"/>
+    <row r="254" ht="15.75" customHeight="1"/>
+    <row r="255" ht="15.75" customHeight="1"/>
+    <row r="256" ht="15.75" customHeight="1"/>
+    <row r="257" ht="15.75" customHeight="1"/>
+    <row r="258" ht="15.75" customHeight="1"/>
+    <row r="259" ht="15.75" customHeight="1"/>
+    <row r="260" ht="15.75" customHeight="1"/>
+    <row r="261" ht="15.75" customHeight="1"/>
+    <row r="262" ht="15.75" customHeight="1"/>
+    <row r="263" ht="15.75" customHeight="1"/>
+    <row r="264" ht="15.75" customHeight="1"/>
+    <row r="265" ht="15.75" customHeight="1"/>
+    <row r="266" ht="15.75" customHeight="1"/>
+    <row r="267" ht="15.75" customHeight="1"/>
+    <row r="268" ht="15.75" customHeight="1"/>
+    <row r="269" ht="15.75" customHeight="1"/>
+    <row r="270" ht="15.75" customHeight="1"/>
+    <row r="271" ht="15.75" customHeight="1"/>
+    <row r="272" ht="15.75" customHeight="1"/>
+    <row r="273" ht="15.75" customHeight="1"/>
+    <row r="274" ht="15.75" customHeight="1"/>
+    <row r="275" ht="15.75" customHeight="1"/>
+    <row r="276" ht="15.75" customHeight="1"/>
+    <row r="277" ht="15.75" customHeight="1"/>
+    <row r="278" ht="15.75" customHeight="1"/>
+    <row r="279" ht="15.75" customHeight="1"/>
+    <row r="280" ht="15.75" customHeight="1"/>
+    <row r="281" ht="15.75" customHeight="1"/>
+    <row r="282" ht="15.75" customHeight="1"/>
+    <row r="283" ht="15.75" customHeight="1"/>
+    <row r="284" ht="15.75" customHeight="1"/>
+    <row r="285" ht="15.75" customHeight="1"/>
+    <row r="286" ht="15.75" customHeight="1"/>
+    <row r="287" ht="15.75" customHeight="1"/>
+    <row r="288" ht="15.75" customHeight="1"/>
+    <row r="289" ht="15.75" customHeight="1"/>
+    <row r="290" ht="15.75" customHeight="1"/>
+    <row r="291" ht="15.75" customHeight="1"/>
+    <row r="292" ht="15.75" customHeight="1"/>
+    <row r="293" ht="15.75" customHeight="1"/>
+    <row r="294" ht="15.75" customHeight="1"/>
+    <row r="295" ht="15.75" customHeight="1"/>
+    <row r="296" ht="15.75" customHeight="1"/>
+    <row r="297" ht="15.75" customHeight="1"/>
+    <row r="298" ht="15.75" customHeight="1"/>
+    <row r="299" ht="15.75" customHeight="1"/>
+    <row r="300" ht="15.75" customHeight="1"/>
+    <row r="301" ht="15.75" customHeight="1"/>
+    <row r="302" ht="15.75" customHeight="1"/>
+    <row r="303" ht="15.75" customHeight="1"/>
+    <row r="304" ht="15.75" customHeight="1"/>
+    <row r="305" ht="15.75" customHeight="1"/>
+    <row r="306" ht="15.75" customHeight="1"/>
+    <row r="307" ht="15.75" customHeight="1"/>
+    <row r="308" ht="15.75" customHeight="1"/>
+    <row r="309" ht="15.75" customHeight="1"/>
+    <row r="310" ht="15.75" customHeight="1"/>
+    <row r="311" ht="15.75" customHeight="1"/>
+    <row r="312" ht="15.75" customHeight="1"/>
+    <row r="313" ht="15.75" customHeight="1"/>
+    <row r="314" ht="15.75" customHeight="1"/>
+    <row r="315" ht="15.75" customHeight="1"/>
+    <row r="316" ht="15.75" customHeight="1"/>
+    <row r="317" ht="15.75" customHeight="1"/>
+    <row r="318" ht="15.75" customHeight="1"/>
+    <row r="319" ht="15.75" customHeight="1"/>
+    <row r="320" ht="15.75" customHeight="1"/>
+    <row r="321" ht="15.75" customHeight="1"/>
+    <row r="322" ht="15.75" customHeight="1"/>
+    <row r="323" ht="15.75" customHeight="1"/>
+    <row r="324" ht="15.75" customHeight="1"/>
+    <row r="325" ht="15.75" customHeight="1"/>
+    <row r="326" ht="15.75" customHeight="1"/>
+    <row r="327" ht="15.75" customHeight="1"/>
+    <row r="328" ht="15.75" customHeight="1"/>
+    <row r="329" ht="15.75" customHeight="1"/>
+    <row r="330" ht="15.75" customHeight="1"/>
+    <row r="331" ht="15.75" customHeight="1"/>
+    <row r="332" ht="15.75" customHeight="1"/>
+    <row r="333" ht="15.75" customHeight="1"/>
+    <row r="334" ht="15.75" customHeight="1"/>
+    <row r="335" ht="15.75" customHeight="1"/>
+    <row r="336" ht="15.75" customHeight="1"/>
+    <row r="337" ht="15.75" customHeight="1"/>
+    <row r="338" ht="15.75" customHeight="1"/>
+    <row r="339" ht="15.75" customHeight="1"/>
+    <row r="340" ht="15.75" customHeight="1"/>
+    <row r="341" ht="15.75" customHeight="1"/>
+    <row r="342" ht="15.75" customHeight="1"/>
+    <row r="343" ht="15.75" customHeight="1"/>
+    <row r="344" ht="15.75" customHeight="1"/>
+    <row r="345" ht="15.75" customHeight="1"/>
+    <row r="346" ht="15.75" customHeight="1"/>
+    <row r="347" ht="15.75" customHeight="1"/>
+    <row r="348" ht="15.75" customHeight="1"/>
+    <row r="349" ht="15.75" customHeight="1"/>
+    <row r="350" ht="15.75" customHeight="1"/>
+    <row r="351" ht="15.75" customHeight="1"/>
+    <row r="352" ht="15.75" customHeight="1"/>
+    <row r="353" ht="15.75" customHeight="1"/>
+    <row r="354" ht="15.75" customHeight="1"/>
+    <row r="355" ht="15.75" customHeight="1"/>
+    <row r="356" ht="15.75" customHeight="1"/>
+    <row r="357" ht="15.75" customHeight="1"/>
+    <row r="358" ht="15.75" customHeight="1"/>
+    <row r="359" ht="15.75" customHeight="1"/>
+    <row r="360" ht="15.75" customHeight="1"/>
+    <row r="361" ht="15.75" customHeight="1"/>
+    <row r="362" ht="15.75" customHeight="1"/>
+    <row r="363" ht="15.75" customHeight="1"/>
+    <row r="364" ht="15.75" customHeight="1"/>
+    <row r="365" ht="15.75" customHeight="1"/>
+    <row r="366" ht="15.75" customHeight="1"/>
+    <row r="367" ht="15.75" customHeight="1"/>
+    <row r="368" ht="15.75" customHeight="1"/>
+    <row r="369" ht="15.75" customHeight="1"/>
+    <row r="370" ht="15.75" customHeight="1"/>
+    <row r="371" ht="15.75" customHeight="1"/>
+    <row r="372" ht="15.75" customHeight="1"/>
+    <row r="373" ht="15.75" customHeight="1"/>
+    <row r="374" ht="15.75" customHeight="1"/>
+    <row r="375" ht="15.75" customHeight="1"/>
+    <row r="376" ht="15.75" customHeight="1"/>
+    <row r="377" ht="15.75" customHeight="1"/>
+    <row r="378" ht="15.75" customHeight="1"/>
+    <row r="379" ht="15.75" customHeight="1"/>
+    <row r="380" ht="15.75" customHeight="1"/>
+    <row r="381" ht="15.75" customHeight="1"/>
+    <row r="382" ht="15.75" customHeight="1"/>
+    <row r="383" ht="15.75" customHeight="1"/>
+    <row r="384" ht="15.75" customHeight="1"/>
+    <row r="385" ht="15.75" customHeight="1"/>
+    <row r="386" ht="15.75" customHeight="1"/>
+    <row r="387" ht="15.75" customHeight="1"/>
+    <row r="388" ht="15.75" customHeight="1"/>
+    <row r="389" ht="15.75" customHeight="1"/>
+    <row r="390" ht="15.75" customHeight="1"/>
+    <row r="391" ht="15.75" customHeight="1"/>
+    <row r="392" ht="15.75" customHeight="1"/>
+    <row r="393" ht="15.75" customHeight="1"/>
+    <row r="394" ht="15.75" customHeight="1"/>
+    <row r="395" ht="15.75" customHeight="1"/>
+    <row r="396" ht="15.75" customHeight="1"/>
+    <row r="397" ht="15.75" customHeight="1"/>
+    <row r="398" ht="15.75" customHeight="1"/>
+    <row r="399" ht="15.75" customHeight="1"/>
+    <row r="400" ht="15.75" customHeight="1"/>
+    <row r="401" ht="15.75" customHeight="1"/>
+    <row r="402" ht="15.75" customHeight="1"/>
+    <row r="403" ht="15.75" customHeight="1"/>
+    <row r="404" ht="15.75" customHeight="1"/>
+    <row r="405" ht="15.75" customHeight="1"/>
+    <row r="406" ht="15.75" customHeight="1"/>
+    <row r="407" ht="15.75" customHeight="1"/>
+    <row r="408" ht="15.75" customHeight="1"/>
+    <row r="409" ht="15.75" customHeight="1"/>
+    <row r="410" ht="15.75" customHeight="1"/>
+    <row r="411" ht="15.75" customHeight="1"/>
+    <row r="412" ht="15.75" customHeight="1"/>
+    <row r="413" ht="15.75" customHeight="1"/>
+    <row r="414" ht="15.75" customHeight="1"/>
+    <row r="415" ht="15.75" customHeight="1"/>
+    <row r="416" ht="15.75" customHeight="1"/>
+    <row r="417" ht="15.75" customHeight="1"/>
+    <row r="418" ht="15.75" customHeight="1"/>
+    <row r="419" ht="15.75" customHeight="1"/>
+    <row r="420" ht="15.75" customHeight="1"/>
+    <row r="421" ht="15.75" customHeight="1"/>
+    <row r="422" ht="15.75" customHeight="1"/>
+    <row r="423" ht="15.75" customHeight="1"/>
+    <row r="424" ht="15.75" customHeight="1"/>
+    <row r="425" ht="15.75" customHeight="1"/>
+    <row r="426" ht="15.75" customHeight="1"/>
+    <row r="427" ht="15.75" customHeight="1"/>
+    <row r="428" ht="15.75" customHeight="1"/>
+    <row r="429" ht="15.75" customHeight="1"/>
+    <row r="430" ht="15.75" customHeight="1"/>
+    <row r="431" ht="15.75" customHeight="1"/>
+    <row r="432" ht="15.75" customHeight="1"/>
+    <row r="433" ht="15.75" customHeight="1"/>
+    <row r="434" ht="15.75" customHeight="1"/>
+    <row r="435" ht="15.75" customHeight="1"/>
+    <row r="436" ht="15.75" customHeight="1"/>
+    <row r="437" ht="15.75" customHeight="1"/>
+    <row r="438" ht="15.75" customHeight="1"/>
+    <row r="439" ht="15.75" customHeight="1"/>
+    <row r="440" ht="15.75" customHeight="1"/>
+    <row r="441" ht="15.75" customHeight="1"/>
+    <row r="442" ht="15.75" customHeight="1"/>
+    <row r="443" ht="15.75" customHeight="1"/>
+    <row r="444" ht="15.75" customHeight="1"/>
+    <row r="445" ht="15.75" customHeight="1"/>
+    <row r="446" ht="15.75" customHeight="1"/>
+    <row r="447" ht="15.75" customHeight="1"/>
+    <row r="448" ht="15.75" customHeight="1"/>
+    <row r="449" ht="15.75" customHeight="1"/>
+    <row r="450" ht="15.75" customHeight="1"/>
+    <row r="451" ht="15.75" customHeight="1"/>
+    <row r="452" ht="15.75" customHeight="1"/>
+    <row r="453" ht="15.75" customHeight="1"/>
+    <row r="454" ht="15.75" customHeight="1"/>
+    <row r="455" ht="15.75" customHeight="1"/>
+    <row r="456" ht="15.75" customHeight="1"/>
+    <row r="457" ht="15.75" customHeight="1"/>
+    <row r="458" ht="15.75" customHeight="1"/>
+    <row r="459" ht="15.75" customHeight="1"/>
+    <row r="460" ht="15.75" customHeight="1"/>
+    <row r="461" ht="15.75" customHeight="1"/>
+    <row r="462" ht="15.75" customHeight="1"/>
+    <row r="463" ht="15.75" customHeight="1"/>
+    <row r="464" ht="15.75" customHeight="1"/>
+    <row r="465" ht="15.75" customHeight="1"/>
+    <row r="466" ht="15.75" customHeight="1"/>
+    <row r="467" ht="15.75" customHeight="1"/>
+    <row r="468" ht="15.75" customHeight="1"/>
+    <row r="469" ht="15.75" customHeight="1"/>
+    <row r="470" ht="15.75" customHeight="1"/>
+    <row r="471" ht="15.75" customHeight="1"/>
+    <row r="472" ht="15.75" customHeight="1"/>
+    <row r="473" ht="15.75" customHeight="1"/>
+    <row r="474" ht="15.75" customHeight="1"/>
+    <row r="475" ht="15.75" customHeight="1"/>
+    <row r="476" ht="15.75" customHeight="1"/>
+    <row r="477" ht="15.75" customHeight="1"/>
+    <row r="478" ht="15.75" customHeight="1"/>
+    <row r="479" ht="15.75" customHeight="1"/>
+    <row r="480" ht="15.75" customHeight="1"/>
+    <row r="481" ht="15.75" customHeight="1"/>
+    <row r="482" ht="15.75" customHeight="1"/>
+    <row r="483" ht="15.75" customHeight="1"/>
+    <row r="484" ht="15.75" customHeight="1"/>
+    <row r="485" ht="15.75" customHeight="1"/>
+    <row r="486" ht="15.75" customHeight="1"/>
+    <row r="487" ht="15.75" customHeight="1"/>
+    <row r="488" ht="15.75" customHeight="1"/>
+    <row r="489" ht="15.75" customHeight="1"/>
+    <row r="490" ht="15.75" customHeight="1"/>
+    <row r="491" ht="15.75" customHeight="1"/>
+    <row r="492" ht="15.75" customHeight="1"/>
+    <row r="493" ht="15.75" customHeight="1"/>
+    <row r="494" ht="15.75" customHeight="1"/>
+    <row r="495" ht="15.75" customHeight="1"/>
+    <row r="496" ht="15.75" customHeight="1"/>
+    <row r="497" ht="15.75" customHeight="1"/>
+    <row r="498" ht="15.75" customHeight="1"/>
+    <row r="499" ht="15.75" customHeight="1"/>
+    <row r="500" ht="15.75" customHeight="1"/>
+    <row r="501" ht="15.75" customHeight="1"/>
+    <row r="502" ht="15.75" customHeight="1"/>
+    <row r="503" ht="15.75" customHeight="1"/>
+    <row r="504" ht="15.75" customHeight="1"/>
+    <row r="505" ht="15.75" customHeight="1"/>
+    <row r="506" ht="15.75" customHeight="1"/>
+    <row r="507" ht="15.75" customHeight="1"/>
+    <row r="508" ht="15.75" customHeight="1"/>
+    <row r="509" ht="15.75" customHeight="1"/>
+    <row r="510" ht="15.75" customHeight="1"/>
+    <row r="511" ht="15.75" customHeight="1"/>
+    <row r="512" ht="15.75" customHeight="1"/>
+    <row r="513" ht="15.75" customHeight="1"/>
+    <row r="514" ht="15.75" customHeight="1"/>
+    <row r="515" ht="15.75" customHeight="1"/>
+    <row r="516" ht="15.75" customHeight="1"/>
+    <row r="517" ht="15.75" customHeight="1"/>
+    <row r="518" ht="15.75" customHeight="1"/>
+    <row r="519" ht="15.75" customHeight="1"/>
+    <row r="520" ht="15.75" customHeight="1"/>
+    <row r="521" ht="15.75" customHeight="1"/>
+    <row r="522" ht="15.75" customHeight="1"/>
+    <row r="523" ht="15.75" customHeight="1"/>
+    <row r="524" ht="15.75" customHeight="1"/>
+    <row r="525" ht="15.75" customHeight="1"/>
+    <row r="526" ht="15.75" customHeight="1"/>
+    <row r="527" ht="15.75" customHeight="1"/>
+    <row r="528" ht="15.75" customHeight="1"/>
+    <row r="529" ht="15.75" customHeight="1"/>
+    <row r="530" ht="15.75" customHeight="1"/>
+    <row r="531" ht="15.75" customHeight="1"/>
+    <row r="532" ht="15.75" customHeight="1"/>
+    <row r="533" ht="15.75" customHeight="1"/>
+    <row r="534" ht="15.75" customHeight="1"/>
+    <row r="535" ht="15.75" customHeight="1"/>
+    <row r="536" ht="15.75" customHeight="1"/>
+    <row r="537" ht="15.75" customHeight="1"/>
+    <row r="538" ht="15.75" customHeight="1"/>
+    <row r="539" ht="15.75" customHeight="1"/>
+    <row r="540" ht="15.75" customHeight="1"/>
+    <row r="541" ht="15.75" customHeight="1"/>
+    <row r="542" ht="15.75" customHeight="1"/>
+    <row r="543" ht="15.75" customHeight="1"/>
+    <row r="544" ht="15.75" customHeight="1"/>
+    <row r="545" ht="15.75" customHeight="1"/>
+    <row r="546" ht="15.75" customHeight="1"/>
+    <row r="547" ht="15.75" customHeight="1"/>
+    <row r="548" ht="15.75" customHeight="1"/>
+    <row r="549" ht="15.75" customHeight="1"/>
+    <row r="550" ht="15.75" customHeight="1"/>
+    <row r="551" ht="15.75" customHeight="1"/>
+    <row r="552" ht="15.75" customHeight="1"/>
+    <row r="553" ht="15.75" customHeight="1"/>
+    <row r="554" ht="15.75" customHeight="1"/>
+    <row r="555" ht="15.75" customHeight="1"/>
+    <row r="556" ht="15.75" customHeight="1"/>
+    <row r="557" ht="15.75" customHeight="1"/>
+    <row r="558" ht="15.75" customHeight="1"/>
+    <row r="559" ht="15.75" customHeight="1"/>
+    <row r="560" ht="15.75" customHeight="1"/>
+    <row r="561" ht="15.75" customHeight="1"/>
+    <row r="562" ht="15.75" customHeight="1"/>
+    <row r="563" ht="15.75" customHeight="1"/>
+    <row r="564" ht="15.75" customHeight="1"/>
+    <row r="565" ht="15.75" customHeight="1"/>
+    <row r="566" ht="15.75" customHeight="1"/>
+    <row r="567" ht="15.75" customHeight="1"/>
+    <row r="568" ht="15.75" customHeight="1"/>
+    <row r="569" ht="15.75" customHeight="1"/>
+    <row r="570" ht="15.75" customHeight="1"/>
+    <row r="571" ht="15.75" customHeight="1"/>
+    <row r="572" ht="15.75" customHeight="1"/>
+    <row r="573" ht="15.75" customHeight="1"/>
+    <row r="574" ht="15.75" customHeight="1"/>
+    <row r="575" ht="15.75" customHeight="1"/>
+    <row r="576" ht="15.75" customHeight="1"/>
+    <row r="577" ht="15.75" customHeight="1"/>
+    <row r="578" ht="15.75" customHeight="1"/>
+    <row r="579" ht="15.75" customHeight="1"/>
+    <row r="580" ht="15.75" customHeight="1"/>
+    <row r="581" ht="15.75" customHeight="1"/>
+    <row r="582" ht="15.75" customHeight="1"/>
+    <row r="583" ht="15.75" customHeight="1"/>
+    <row r="584" ht="15.75" customHeight="1"/>
+    <row r="585" ht="15.75" customHeight="1"/>
+    <row r="586" ht="15.75" customHeight="1"/>
+    <row r="587" ht="15.75" customHeight="1"/>
+    <row r="588" ht="15.75" customHeight="1"/>
+    <row r="589" ht="15.75" customHeight="1"/>
+    <row r="590" ht="15.75" customHeight="1"/>
+    <row r="591" ht="15.75" customHeight="1"/>
+    <row r="592" ht="15.75" customHeight="1"/>
+    <row r="593" ht="15.75" customHeight="1"/>
+    <row r="594" ht="15.75" customHeight="1"/>
+    <row r="595" ht="15.75" customHeight="1"/>
+    <row r="596" ht="15.75" customHeight="1"/>
+    <row r="597" ht="15.75" customHeight="1"/>
+    <row r="598" ht="15.75" customHeight="1"/>
+    <row r="599" ht="15.75" customHeight="1"/>
+    <row r="600" ht="15.75" customHeight="1"/>
+    <row r="601" ht="15.75" customHeight="1"/>
+    <row r="602" ht="15.75" customHeight="1"/>
+    <row r="603" ht="15.75" customHeight="1"/>
+    <row r="604" ht="15.75" customHeight="1"/>
+    <row r="605" ht="15.75" customHeight="1"/>
+    <row r="606" ht="15.75" customHeight="1"/>
+    <row r="607" ht="15.75" customHeight="1"/>
+    <row r="608" ht="15.75" customHeight="1"/>
+    <row r="609" ht="15.75" customHeight="1"/>
+    <row r="610" ht="15.75" customHeight="1"/>
+    <row r="611" ht="15.75" customHeight="1"/>
+    <row r="612" ht="15.75" customHeight="1"/>
+    <row r="613" ht="15.75" customHeight="1"/>
+    <row r="614" ht="15.75" customHeight="1"/>
+    <row r="615" ht="15.75" customHeight="1"/>
+    <row r="616" ht="15.75" customHeight="1"/>
+    <row r="617" ht="15.75" customHeight="1"/>
+    <row r="618" ht="15.75" customHeight="1"/>
+    <row r="619" ht="15.75" customHeight="1"/>
+    <row r="620" ht="15.75" customHeight="1"/>
+    <row r="621" ht="15.75" customHeight="1"/>
+    <row r="622" ht="15.75" customHeight="1"/>
+    <row r="623" ht="15.75" customHeight="1"/>
+    <row r="624" ht="15.75" customHeight="1"/>
+    <row r="625" ht="15.75" customHeight="1"/>
+    <row r="626" ht="15.75" customHeight="1"/>
+    <row r="627" ht="15.75" customHeight="1"/>
+    <row r="628" ht="15.75" customHeight="1"/>
+    <row r="629" ht="15.75" customHeight="1"/>
+    <row r="630" ht="15.75" customHeight="1"/>
+    <row r="631" ht="15.75" customHeight="1"/>
+    <row r="632" ht="15.75" customHeight="1"/>
+    <row r="633" ht="15.75" customHeight="1"/>
+    <row r="634" ht="15.75" customHeight="1"/>
+    <row r="635" ht="15.75" customHeight="1"/>
+    <row r="636" ht="15.75" customHeight="1"/>
+    <row r="637" ht="15.75" customHeight="1"/>
+    <row r="638" ht="15.75" customHeight="1"/>
+    <row r="639" ht="15.75" customHeight="1"/>
+    <row r="640" ht="15.75" customHeight="1"/>
+    <row r="641" ht="15.75" customHeight="1"/>
+    <row r="642" ht="15.75" customHeight="1"/>
+    <row r="643" ht="15.75" customHeight="1"/>
+    <row r="644" ht="15.75" customHeight="1"/>
+    <row r="645" ht="15.75" customHeight="1"/>
+    <row r="646" ht="15.75" customHeight="1"/>
+    <row r="647" ht="15.75" customHeight="1"/>
+    <row r="648" ht="15.75" customHeight="1"/>
+    <row r="649" ht="15.75" customHeight="1"/>
+    <row r="650" ht="15.75" customHeight="1"/>
+    <row r="651" ht="15.75" customHeight="1"/>
+    <row r="652" ht="15.75" customHeight="1"/>
+    <row r="653" ht="15.75" customHeight="1"/>
+    <row r="654" ht="15.75" customHeight="1"/>
+    <row r="655" ht="15.75" customHeight="1"/>
+    <row r="656" ht="15.75" customHeight="1"/>
+    <row r="657" ht="15.75" customHeight="1"/>
+    <row r="658" ht="15.75" customHeight="1"/>
+    <row r="659" ht="15.75" customHeight="1"/>
+    <row r="660" ht="15.75" customHeight="1"/>
+    <row r="661" ht="15.75" customHeight="1"/>
+    <row r="662" ht="15.75" customHeight="1"/>
+    <row r="663" ht="15.75" customHeight="1"/>
+    <row r="664" ht="15.75" customHeight="1"/>
+    <row r="665" ht="15.75" customHeight="1"/>
+    <row r="666" ht="15.75" customHeight="1"/>
+    <row r="667" ht="15.75" customHeight="1"/>
+    <row r="668" ht="15.75" customHeight="1"/>
+    <row r="669" ht="15.75" customHeight="1"/>
+    <row r="670" ht="15.75" customHeight="1"/>
+    <row r="671" ht="15.75" customHeight="1"/>
+    <row r="672" ht="15.75" customHeight="1"/>
+    <row r="673" ht="15.75" customHeight="1"/>
+    <row r="674" ht="15.75" customHeight="1"/>
+    <row r="675" ht="15.75" customHeight="1"/>
+    <row r="676" ht="15.75" customHeight="1"/>
+    <row r="677" ht="15.75" customHeight="1"/>
+    <row r="678" ht="15.75" customHeight="1"/>
+    <row r="679" ht="15.75" customHeight="1"/>
+    <row r="680" ht="15.75" customHeight="1"/>
+    <row r="681" ht="15.75" customHeight="1"/>
+    <row r="682" ht="15.75" customHeight="1"/>
+    <row r="683" ht="15.75" customHeight="1"/>
+    <row r="684" ht="15.75" customHeight="1"/>
+    <row r="685" ht="15.75" customHeight="1"/>
+    <row r="686" ht="15.75" customHeight="1"/>
+    <row r="687" ht="15.75" customHeight="1"/>
+    <row r="688" ht="15.75" customHeight="1"/>
+    <row r="689" ht="15.75" customHeight="1"/>
+    <row r="690" ht="15.75" customHeight="1"/>
+    <row r="691" ht="15.75" customHeight="1"/>
+    <row r="692" ht="15.75" customHeight="1"/>
+    <row r="693" ht="15.75" customHeight="1"/>
+    <row r="694" ht="15.75" customHeight="1"/>
+    <row r="695" ht="15.75" customHeight="1"/>
+    <row r="696" ht="15.75" customHeight="1"/>
+    <row r="697" ht="15.75" customHeight="1"/>
+    <row r="698" ht="15.75" customHeight="1"/>
+    <row r="699" ht="15.75" customHeight="1"/>
+    <row r="700" ht="15.75" customHeight="1"/>
+    <row r="701" ht="15.75" customHeight="1"/>
+    <row r="702" ht="15.75" customHeight="1"/>
+    <row r="703" ht="15.75" customHeight="1"/>
+    <row r="704" ht="15.75" customHeight="1"/>
+    <row r="705" ht="15.75" customHeight="1"/>
+    <row r="706" ht="15.75" customHeight="1"/>
+    <row r="707" ht="15.75" customHeight="1"/>
+    <row r="708" ht="15.75" customHeight="1"/>
+    <row r="709" ht="15.75" customHeight="1"/>
+    <row r="710" ht="15.75" customHeight="1"/>
+    <row r="711" ht="15.75" customHeight="1"/>
+    <row r="712" ht="15.75" customHeight="1"/>
+    <row r="713" ht="15.75" customHeight="1"/>
+    <row r="714" ht="15.75" customHeight="1"/>
+    <row r="715" ht="15.75" customHeight="1"/>
+    <row r="716" ht="15.75" customHeight="1"/>
+    <row r="717" ht="15.75" customHeight="1"/>
+    <row r="718" ht="15.75" customHeight="1"/>
+    <row r="719" ht="15.75" customHeight="1"/>
+    <row r="720" ht="15.75" customHeight="1"/>
+    <row r="721" ht="15.75" customHeight="1"/>
+    <row r="722" ht="15.75" customHeight="1"/>
+    <row r="723" ht="15.75" customHeight="1"/>
+    <row r="724" ht="15.75" customHeight="1"/>
+    <row r="725" ht="15.75" customHeight="1"/>
+    <row r="726" ht="15.75" customHeight="1"/>
+    <row r="727" ht="15.75" customHeight="1"/>
+    <row r="728" ht="15.75" customHeight="1"/>
+    <row r="729" ht="15.75" customHeight="1"/>
+    <row r="730" ht="15.75" customHeight="1"/>
+    <row r="731" ht="15.75" customHeight="1"/>
+    <row r="732" ht="15.75" customHeight="1"/>
+    <row r="733" ht="15.75" customHeight="1"/>
+    <row r="734" ht="15.75" customHeight="1"/>
+    <row r="735" ht="15.75" customHeight="1"/>
+    <row r="736" ht="15.75" customHeight="1"/>
+    <row r="737" ht="15.75" customHeight="1"/>
+    <row r="738" ht="15.75" customHeight="1"/>
+    <row r="739" ht="15.75" customHeight="1"/>
+    <row r="740" ht="15.75" customHeight="1"/>
+    <row r="741" ht="15.75" customHeight="1"/>
+    <row r="742" ht="15.75" customHeight="1"/>
+    <row r="743" ht="15.75" customHeight="1"/>
+    <row r="744" ht="15.75" customHeight="1"/>
+    <row r="745" ht="15.75" customHeight="1"/>
+    <row r="746" ht="15.75" customHeight="1"/>
+    <row r="747" ht="15.75" customHeight="1"/>
+    <row r="748" ht="15.75" customHeight="1"/>
+    <row r="749" ht="15.75" customHeight="1"/>
+    <row r="750" ht="15.75" customHeight="1"/>
+    <row r="751" ht="15.75" customHeight="1"/>
+    <row r="752" ht="15.75" customHeight="1"/>
+    <row r="753" ht="15.75" customHeight="1"/>
+    <row r="754" ht="15.75" customHeight="1"/>
+    <row r="755" ht="15.75" customHeight="1"/>
+    <row r="756" ht="15.75" customHeight="1"/>
+    <row r="757" ht="15.75" customHeight="1"/>
+    <row r="758" ht="15.75" customHeight="1"/>
+    <row r="759" ht="15.75" customHeight="1"/>
+    <row r="760" ht="15.75" customHeight="1"/>
+    <row r="761" ht="15.75" customHeight="1"/>
+    <row r="762" ht="15.75" customHeight="1"/>
+    <row r="763" ht="15.75" customHeight="1"/>
+    <row r="764" ht="15.75" customHeight="1"/>
+    <row r="765" ht="15.75" customHeight="1"/>
+    <row r="766" ht="15.75" customHeight="1"/>
+    <row r="767" ht="15.75" customHeight="1"/>
+    <row r="768" ht="15.75" customHeight="1"/>
+    <row r="769" ht="15.75" customHeight="1"/>
+    <row r="770" ht="15.75" customHeight="1"/>
+    <row r="771" ht="15.75" customHeight="1"/>
+    <row r="772" ht="15.75" customHeight="1"/>
+    <row r="773" ht="15.75" customHeight="1"/>
+    <row r="774" ht="15.75" customHeight="1"/>
+    <row r="775" ht="15.75" customHeight="1"/>
+    <row r="776" ht="15.75" customHeight="1"/>
+    <row r="777" ht="15.75" customHeight="1"/>
+    <row r="778" ht="15.75" customHeight="1"/>
+    <row r="779" ht="15.75" customHeight="1"/>
+    <row r="780" ht="15.75" customHeight="1"/>
+    <row r="781" ht="15.75" customHeight="1"/>
+    <row r="782" ht="15.75" customHeight="1"/>
+    <row r="783" ht="15.75" customHeight="1"/>
+    <row r="784" ht="15.75" customHeight="1"/>
+    <row r="785" ht="15.75" customHeight="1"/>
+    <row r="786" ht="15.75" customHeight="1"/>
+    <row r="787" ht="15.75" customHeight="1"/>
+    <row r="788" ht="15.75" customHeight="1"/>
+    <row r="789" ht="15.75" customHeight="1"/>
+    <row r="790" ht="15.75" customHeight="1"/>
+    <row r="791" ht="15.75" customHeight="1"/>
+    <row r="792" ht="15.75" customHeight="1"/>
+    <row r="793" ht="15.75" customHeight="1"/>
+    <row r="794" ht="15.75" customHeight="1"/>
+    <row r="795" ht="15.75" customHeight="1"/>
+    <row r="796" ht="15.75" customHeight="1"/>
+    <row r="797" ht="15.75" customHeight="1"/>
+    <row r="798" ht="15.75" customHeight="1"/>
+    <row r="799" ht="15.75" customHeight="1"/>
+    <row r="800" ht="15.75" customHeight="1"/>
+    <row r="801" ht="15.75" customHeight="1"/>
+    <row r="802" ht="15.75" customHeight="1"/>
+    <row r="803" ht="15.75" customHeight="1"/>
+    <row r="804" ht="15.75" customHeight="1"/>
+    <row r="805" ht="15.75" customHeight="1"/>
+    <row r="806" ht="15.75" customHeight="1"/>
+    <row r="807" ht="15.75" customHeight="1"/>
+    <row r="808" ht="15.75" customHeight="1"/>
+    <row r="809" ht="15.75" customHeight="1"/>
+    <row r="810" ht="15.75" customHeight="1"/>
+    <row r="811" ht="15.75" customHeight="1"/>
+    <row r="812" ht="15.75" customHeight="1"/>
+    <row r="813" ht="15.75" customHeight="1"/>
+    <row r="814" ht="15.75" customHeight="1"/>
+    <row r="815" ht="15.75" customHeight="1"/>
+    <row r="816" ht="15.75" customHeight="1"/>
+    <row r="817" ht="15.75" customHeight="1"/>
+    <row r="818" ht="15.75" customHeight="1"/>
+    <row r="819" ht="15.75" customHeight="1"/>
+    <row r="820" ht="15.75" customHeight="1"/>
+    <row r="821" ht="15.75" customHeight="1"/>
+    <row r="822" ht="15.75" customHeight="1"/>
+    <row r="823" ht="15.75" customHeight="1"/>
+    <row r="824" ht="15.75" customHeight="1"/>
+    <row r="825" ht="15.75" customHeight="1"/>
+    <row r="826" ht="15.75" customHeight="1"/>
+    <row r="827" ht="15.75" customHeight="1"/>
+    <row r="828" ht="15.75" customHeight="1"/>
+    <row r="829" ht="15.75" customHeight="1"/>
+    <row r="830" ht="15.75" customHeight="1"/>
+    <row r="831" ht="15.75" customHeight="1"/>
+    <row r="832" ht="15.75" customHeight="1"/>
+    <row r="833" ht="15.75" customHeight="1"/>
+    <row r="834" ht="15.75" customHeight="1"/>
+    <row r="835" ht="15.75" customHeight="1"/>
+    <row r="836" ht="15.75" customHeight="1"/>
+    <row r="837" ht="15.75" customHeight="1"/>
+    <row r="838" ht="15.75" customHeight="1"/>
+    <row r="839" ht="15.75" customHeight="1"/>
+    <row r="840" ht="15.75" customHeight="1"/>
+    <row r="841" ht="15.75" customHeight="1"/>
+    <row r="842" ht="15.75" customHeight="1"/>
+    <row r="843" ht="15.75" customHeight="1"/>
+    <row r="844" ht="15.75" customHeight="1"/>
+    <row r="845" ht="15.75" customHeight="1"/>
+    <row r="846" ht="15.75" customHeight="1"/>
+    <row r="847" ht="15.75" customHeight="1"/>
+    <row r="848" ht="15.75" customHeight="1"/>
+    <row r="849" ht="15.75" customHeight="1"/>
+    <row r="850" ht="15.75" customHeight="1"/>
+    <row r="851" ht="15.75" customHeight="1"/>
+    <row r="852" ht="15.75" customHeight="1"/>
+    <row r="853" ht="15.75" customHeight="1"/>
+    <row r="854" ht="15.75" customHeight="1"/>
+    <row r="855" ht="15.75" customHeight="1"/>
+    <row r="856" ht="15.75" customHeight="1"/>
+    <row r="857" ht="15.75" customHeight="1"/>
+    <row r="858" ht="15.75" customHeight="1"/>
+    <row r="859" ht="15.75" customHeight="1"/>
+    <row r="860" ht="15.75" customHeight="1"/>
+    <row r="861" ht="15.75" customHeight="1"/>
+    <row r="862" ht="15.75" customHeight="1"/>
+    <row r="863" ht="15.75" customHeight="1"/>
+    <row r="864" ht="15.75" customHeight="1"/>
+    <row r="865" ht="15.75" customHeight="1"/>
+    <row r="866" ht="15.75" customHeight="1"/>
+    <row r="867" ht="15.75" customHeight="1"/>
+    <row r="868" ht="15.75" customHeight="1"/>
+    <row r="869" ht="15.75" customHeight="1"/>
+    <row r="870" ht="15.75" customHeight="1"/>
+    <row r="871" ht="15.75" customHeight="1"/>
+    <row r="872" ht="15.75" customHeight="1"/>
+    <row r="873" ht="15.75" customHeight="1"/>
+    <row r="874" ht="15.75" customHeight="1"/>
+    <row r="875" ht="15.75" customHeight="1"/>
+    <row r="876" ht="15.75" customHeight="1"/>
+    <row r="877" ht="15.75" customHeight="1"/>
+    <row r="878" ht="15.75" customHeight="1"/>
+    <row r="879" ht="15.75" customHeight="1"/>
+    <row r="880" ht="15.75" customHeight="1"/>
+    <row r="881" ht="15.75" customHeight="1"/>
+    <row r="882" ht="15.75" customHeight="1"/>
+    <row r="883" ht="15.75" customHeight="1"/>
+    <row r="884" ht="15.75" customHeight="1"/>
+    <row r="885" ht="15.75" customHeight="1"/>
+    <row r="886" ht="15.75" customHeight="1"/>
+    <row r="887" ht="15.75" customHeight="1"/>
+    <row r="888" ht="15.75" customHeight="1"/>
+    <row r="889" ht="15.75" customHeight="1"/>
+    <row r="890" ht="15.75" customHeight="1"/>
+    <row r="891" ht="15.75" customHeight="1"/>
+    <row r="892" ht="15.75" customHeight="1"/>
+    <row r="893" ht="15.75" customHeight="1"/>
+    <row r="894" ht="15.75" customHeight="1"/>
+    <row r="895" ht="15.75" customHeight="1"/>
+    <row r="896" ht="15.75" customHeight="1"/>
+    <row r="897" ht="15.75" customHeight="1"/>
+    <row r="898" ht="15.75" customHeight="1"/>
+    <row r="899" ht="15.75" customHeight="1"/>
+    <row r="900" ht="15.75" customHeight="1"/>
+    <row r="901" ht="15.75" customHeight="1"/>
+    <row r="902" ht="15.75" customHeight="1"/>
+    <row r="903" ht="15.75" customHeight="1"/>
+    <row r="904" ht="15.75" customHeight="1"/>
+    <row r="905" ht="15.75" customHeight="1"/>
+    <row r="906" ht="15.75" customHeight="1"/>
+    <row r="907" ht="15.75" customHeight="1"/>
+    <row r="908" ht="15.75" customHeight="1"/>
+    <row r="909" ht="15.75" customHeight="1"/>
+    <row r="910" ht="15.75" customHeight="1"/>
+    <row r="911" ht="15.75" customHeight="1"/>
+    <row r="912" ht="15.75" customHeight="1"/>
+    <row r="913" ht="15.75" customHeight="1"/>
+    <row r="914" ht="15.75" customHeight="1"/>
+    <row r="915" ht="15.75" customHeight="1"/>
+    <row r="916" ht="15.75" customHeight="1"/>
+    <row r="917" ht="15.75" customHeight="1"/>
+    <row r="918" ht="15.75" customHeight="1"/>
+    <row r="919" ht="15.75" customHeight="1"/>
+    <row r="920" ht="15.75" customHeight="1"/>
+    <row r="921" ht="15.75" customHeight="1"/>
+    <row r="922" ht="15.75" customHeight="1"/>
+    <row r="923" ht="15.75" customHeight="1"/>
+    <row r="924" ht="15.75" customHeight="1"/>
+    <row r="925" ht="15.75" customHeight="1"/>
+    <row r="926" ht="15.75" customHeight="1"/>
+    <row r="927" ht="15.75" customHeight="1"/>
+    <row r="928" ht="15.75" customHeight="1"/>
+    <row r="929" ht="15.75" customHeight="1"/>
+    <row r="930" ht="15.75" customHeight="1"/>
+    <row r="931" ht="15.75" customHeight="1"/>
+    <row r="932" ht="15.75" customHeight="1"/>
+    <row r="933" ht="15.75" customHeight="1"/>
+    <row r="934" ht="15.75" customHeight="1"/>
+    <row r="935" ht="15.75" customHeight="1"/>
+    <row r="936" ht="15.75" customHeight="1"/>
+    <row r="937" ht="15.75" customHeight="1"/>
+    <row r="938" ht="15.75" customHeight="1"/>
+    <row r="939" ht="15.75" customHeight="1"/>
+    <row r="940" ht="15.75" customHeight="1"/>
+    <row r="941" ht="15.75" customHeight="1"/>
+    <row r="942" ht="15.75" customHeight="1"/>
+    <row r="943" ht="15.75" customHeight="1"/>
+    <row r="944" ht="15.75" customHeight="1"/>
+    <row r="945" ht="15.75" customHeight="1"/>
+    <row r="946" ht="15.75" customHeight="1"/>
+    <row r="947" ht="15.75" customHeight="1"/>
+    <row r="948" ht="15.75" customHeight="1"/>
+    <row r="949" ht="15.75" customHeight="1"/>
+    <row r="950" ht="15.75" customHeight="1"/>
+    <row r="951" ht="15.75" customHeight="1"/>
+    <row r="952" ht="15.75" customHeight="1"/>
+    <row r="953" ht="15.75" customHeight="1"/>
+    <row r="954" ht="15.75" customHeight="1"/>
+    <row r="955" ht="15.75" customHeight="1"/>
+    <row r="956" ht="15.75" customHeight="1"/>
+    <row r="957" ht="15.75" customHeight="1"/>
+    <row r="958" ht="15.75" customHeight="1"/>
+    <row r="959" ht="15.75" customHeight="1"/>
+    <row r="960" ht="15.75" customHeight="1"/>
+    <row r="961" ht="15.75" customHeight="1"/>
+    <row r="962" ht="15.75" customHeight="1"/>
+    <row r="963" ht="15.75" customHeight="1"/>
+    <row r="964" ht="15.75" customHeight="1"/>
+    <row r="965" ht="15.75" customHeight="1"/>
+    <row r="966" ht="15.75" customHeight="1"/>
+    <row r="967" ht="15.75" customHeight="1"/>
+    <row r="968" ht="15.75" customHeight="1"/>
+    <row r="969" ht="15.75" customHeight="1"/>
+    <row r="970" ht="15.75" customHeight="1"/>
+    <row r="971" ht="15.75" customHeight="1"/>
+    <row r="972" ht="15.75" customHeight="1"/>
+    <row r="973" ht="15.75" customHeight="1"/>
+    <row r="974" ht="15.75" customHeight="1"/>
+    <row r="975" ht="15.75" customHeight="1"/>
+    <row r="976" ht="15.75" customHeight="1"/>
+    <row r="977" ht="15.75" customHeight="1"/>
+    <row r="978" ht="15.75" customHeight="1"/>
+    <row r="979" ht="15.75" customHeight="1"/>
+    <row r="980" ht="15.75" customHeight="1"/>
+    <row r="981" ht="15.75" customHeight="1"/>
+    <row r="982" ht="15.75" customHeight="1"/>
+    <row r="983" ht="15.75" customHeight="1"/>
+    <row r="984" ht="15.75" customHeight="1"/>
+    <row r="985" ht="15.75" customHeight="1"/>
+    <row r="986" ht="15.75" customHeight="1"/>
+    <row r="987" ht="15.75" customHeight="1"/>
+    <row r="988" ht="15.75" customHeight="1"/>
+    <row r="989" ht="15.75" customHeight="1"/>
+    <row r="990" ht="15.75" customHeight="1"/>
+    <row r="991" ht="15.75" customHeight="1"/>
+    <row r="992" ht="15.75" customHeight="1"/>
+    <row r="993" ht="15.75" customHeight="1"/>
+    <row r="994" ht="15.75" customHeight="1"/>
+    <row r="995" ht="15.75" customHeight="1"/>
+    <row r="996" ht="15.75" customHeight="1"/>
+    <row r="997" ht="15.75" customHeight="1"/>
+    <row r="998" ht="15.75" customHeight="1"/>
+    <row r="999" ht="15.75" customHeight="1"/>
+    <row r="1000" ht="15.75" customHeight="1"/>
+  </sheetData>
+  <mergeCells count="21">
+    <mergeCell ref="L15:L17"/>
+    <mergeCell ref="M15:O17"/>
+    <mergeCell ref="C19:D20"/>
+    <mergeCell ref="E19:O20"/>
+    <mergeCell ref="C22:D24"/>
+    <mergeCell ref="E22:H24"/>
+    <mergeCell ref="J22:K24"/>
+    <mergeCell ref="L22:O24"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="C15:C17"/>
+    <mergeCell ref="D15:E17"/>
+    <mergeCell ref="G15:G17"/>
+    <mergeCell ref="H15:J17"/>
+    <mergeCell ref="B6:P6"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="H12:I12"/>
+  </mergeCells>
+  <conditionalFormatting sqref="H10:I11">
+    <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
+      <formula>"Atrasado"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H10:I11">
+    <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
+      <formula>"Terminado"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H10:I11">
+    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
+      <formula>"En proceso"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H10:I11">
+    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
+      <formula>"No Iniciado"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <printOptions horizontalCentered="1"/>
+  <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0" footer="0"/>
+  <pageSetup paperSize="9" orientation="landscape"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{C7464F15-59D8-447C-B97A-3A303B371DF5}">
+          <x14:formula1>
+            <xm:f>'Formato descripción HU'!$B$6:$B$23</xm:f>
+          </x14:formula1>
+          <xm:sqref>C10:C11</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71CA9216-54C8-477A-B842-BC85877331BF}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A2:Z1000"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="S15" sqref="S15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1"/>
+  <cols>
+    <col min="1" max="1" width="9.375" style="39" customWidth="1"/>
+    <col min="2" max="2" width="2.625" style="39" customWidth="1"/>
+    <col min="3" max="15" width="10.625" style="39" customWidth="1"/>
+    <col min="16" max="16" width="2.625" style="39" customWidth="1"/>
+    <col min="17" max="26" width="9.375" style="39" customWidth="1"/>
+    <col min="27" max="16384" width="12.625" style="39"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:26" ht="15" hidden="1" customHeight="1"/>
+    <row r="3" spans="1:26" ht="15" hidden="1" customHeight="1"/>
+    <row r="4" spans="1:26" ht="14.45" hidden="1">
+      <c r="C4" s="15"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="16"/>
+    </row>
+    <row r="5" spans="1:26" ht="14.45" hidden="1">
+      <c r="C5" s="15"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="16"/>
+    </row>
+    <row r="6" spans="1:26" ht="39.75" customHeight="1">
+      <c r="B6" s="88" t="s">
+        <v>91</v>
+      </c>
+      <c r="C6" s="63"/>
+      <c r="D6" s="63"/>
+      <c r="E6" s="63"/>
+      <c r="F6" s="63"/>
+      <c r="G6" s="63"/>
+      <c r="H6" s="63"/>
+      <c r="I6" s="63"/>
+      <c r="J6" s="63"/>
+      <c r="K6" s="63"/>
+      <c r="L6" s="63"/>
+      <c r="M6" s="63"/>
+      <c r="N6" s="63"/>
+      <c r="O6" s="63"/>
+      <c r="P6" s="64"/>
+    </row>
+    <row r="7" spans="1:26" ht="9.75" customHeight="1">
+      <c r="A7" s="17"/>
+      <c r="B7" s="17"/>
+      <c r="C7" s="18"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="18"/>
+      <c r="G7" s="18"/>
+      <c r="H7" s="18"/>
+      <c r="I7" s="18"/>
+      <c r="J7" s="18"/>
+      <c r="K7" s="18"/>
+      <c r="L7" s="18"/>
+      <c r="M7" s="18"/>
+      <c r="N7" s="18"/>
+      <c r="O7" s="18"/>
+      <c r="P7" s="17"/>
+      <c r="Q7" s="17"/>
+      <c r="R7" s="17"/>
+      <c r="S7" s="17"/>
+      <c r="T7" s="17"/>
+      <c r="U7" s="17"/>
+      <c r="V7" s="17"/>
+      <c r="W7" s="17"/>
+      <c r="X7" s="17"/>
+      <c r="Y7" s="17"/>
+      <c r="Z7" s="17"/>
+    </row>
+    <row r="8" spans="1:26" ht="9.75" customHeight="1">
+      <c r="B8" s="32"/>
+      <c r="C8" s="33"/>
+      <c r="D8" s="33"/>
+      <c r="E8" s="33"/>
+      <c r="F8" s="34"/>
+      <c r="G8" s="35"/>
+      <c r="H8" s="35"/>
+      <c r="I8" s="35"/>
+      <c r="J8" s="35"/>
+      <c r="K8" s="35"/>
+      <c r="L8" s="35"/>
+      <c r="M8" s="35"/>
+      <c r="N8" s="35"/>
+      <c r="O8" s="35"/>
+      <c r="P8" s="36"/>
+      <c r="Q8" s="17"/>
+    </row>
+    <row r="9" spans="1:26" ht="30" customHeight="1">
+      <c r="B9" s="37"/>
+      <c r="C9" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" s="20"/>
+      <c r="E9" s="83" t="s">
+        <v>92</v>
+      </c>
+      <c r="F9" s="64"/>
+      <c r="G9" s="20"/>
+      <c r="H9" s="83" t="s">
+        <v>11</v>
+      </c>
+      <c r="I9" s="64"/>
+      <c r="J9" s="21"/>
+      <c r="K9" s="21"/>
+      <c r="L9" s="21"/>
+      <c r="M9" s="21"/>
+      <c r="N9" s="21"/>
+      <c r="O9" s="21"/>
+      <c r="P9" s="38"/>
+      <c r="Q9" s="17"/>
+    </row>
+    <row r="10" spans="1:26" ht="30" customHeight="1">
+      <c r="B10" s="37"/>
+      <c r="C10" s="26" t="s">
+        <v>77</v>
+      </c>
+      <c r="D10" s="22"/>
+      <c r="E10" s="84" t="str">
+        <f>VLOOKUP(C10,'Formato descripción HU'!B6:O23,5,0)</f>
+        <v>Sistema / Coordinación</v>
+      </c>
+      <c r="F10" s="64"/>
+      <c r="G10" s="23"/>
+      <c r="H10" s="84" t="str">
+        <f>VLOOKUP(C10,'Formato descripción HU'!B6:O23,11,0)</f>
+        <v>Conflictivo</v>
+      </c>
+      <c r="I10" s="64"/>
+      <c r="J10" s="23"/>
+      <c r="K10" s="21"/>
+      <c r="L10" s="21"/>
+      <c r="M10" s="21"/>
+      <c r="N10" s="21"/>
+      <c r="O10" s="21"/>
+      <c r="P10" s="38"/>
+      <c r="Q10" s="17"/>
+    </row>
+    <row r="11" spans="1:26" ht="9.75" customHeight="1">
+      <c r="A11" s="17"/>
+      <c r="B11" s="37"/>
+      <c r="C11" s="24"/>
+      <c r="D11" s="22"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="25"/>
+      <c r="G11" s="23"/>
+      <c r="H11" s="25"/>
+      <c r="I11" s="25"/>
+      <c r="J11" s="23"/>
+      <c r="K11" s="25"/>
+      <c r="L11" s="25"/>
+      <c r="M11" s="21"/>
+      <c r="N11" s="25"/>
+      <c r="O11" s="25"/>
+      <c r="P11" s="38"/>
+      <c r="Q11" s="17"/>
+      <c r="R11" s="17"/>
+      <c r="S11" s="17"/>
+      <c r="T11" s="17"/>
+      <c r="U11" s="17"/>
+      <c r="V11" s="17"/>
+      <c r="W11" s="17"/>
+      <c r="X11" s="17"/>
+      <c r="Y11" s="17"/>
+      <c r="Z11" s="17"/>
+    </row>
+    <row r="12" spans="1:26" ht="30" customHeight="1">
+      <c r="A12" s="17"/>
+      <c r="B12" s="37"/>
+      <c r="C12" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="D12" s="22"/>
+      <c r="E12" s="83" t="s">
+        <v>10</v>
+      </c>
+      <c r="F12" s="64"/>
+      <c r="G12" s="23"/>
+      <c r="H12" s="83" t="s">
+        <v>94</v>
+      </c>
+      <c r="I12" s="64"/>
+      <c r="J12" s="23"/>
+      <c r="K12" s="25"/>
+      <c r="L12" s="25"/>
+      <c r="M12" s="21"/>
+      <c r="N12" s="25"/>
+      <c r="O12" s="25"/>
+      <c r="P12" s="38"/>
+      <c r="Q12" s="17"/>
+      <c r="R12" s="17"/>
+      <c r="S12" s="17"/>
+      <c r="T12" s="17"/>
+      <c r="U12" s="17"/>
+      <c r="V12" s="17"/>
+      <c r="W12" s="17"/>
+      <c r="X12" s="17"/>
+      <c r="Y12" s="17"/>
+      <c r="Z12" s="17"/>
+    </row>
+    <row r="13" spans="1:26" ht="30" customHeight="1">
+      <c r="A13" s="17"/>
+      <c r="B13" s="37"/>
+      <c r="C13" s="26">
+        <f>VLOOKUP('Historia de Usuario RF-07'!C10,'Formato descripción HU'!B6:O23,8,0)</f>
+        <v>12</v>
+      </c>
+      <c r="D13" s="22"/>
+      <c r="E13" s="84" t="str">
+        <f>VLOOKUP(C10,'Formato descripción HU'!B6:O23,10,0)</f>
+        <v>Alta</v>
+      </c>
+      <c r="F13" s="64"/>
+      <c r="G13" s="23"/>
+      <c r="H13" s="84" t="str">
+        <f>VLOOKUP(C10,'Formato descripción HU'!B6:O23,7,0)</f>
+        <v>Stefany Díaz</v>
+      </c>
+      <c r="I13" s="64"/>
+      <c r="J13" s="23"/>
+      <c r="K13" s="25"/>
+      <c r="L13" s="25"/>
+      <c r="M13" s="21"/>
+      <c r="N13" s="25"/>
+      <c r="O13" s="25"/>
+      <c r="P13" s="38"/>
+      <c r="Q13" s="17"/>
+      <c r="R13" s="17"/>
+      <c r="S13" s="17"/>
+      <c r="T13" s="17"/>
+      <c r="U13" s="17"/>
+      <c r="V13" s="17"/>
+      <c r="W13" s="17"/>
+      <c r="X13" s="17"/>
+      <c r="Y13" s="17"/>
+      <c r="Z13" s="17"/>
+    </row>
+    <row r="14" spans="1:26" ht="9.75" customHeight="1">
+      <c r="A14" s="17"/>
+      <c r="B14" s="37"/>
+      <c r="C14" s="21"/>
+      <c r="D14" s="22"/>
+      <c r="E14" s="21"/>
+      <c r="F14" s="21"/>
+      <c r="G14" s="23"/>
+      <c r="H14" s="23"/>
+      <c r="I14" s="21"/>
+      <c r="J14" s="21"/>
+      <c r="K14" s="21"/>
+      <c r="L14" s="21"/>
+      <c r="M14" s="21"/>
+      <c r="N14" s="21"/>
+      <c r="O14" s="21"/>
+      <c r="P14" s="38"/>
+      <c r="Q14" s="17"/>
+      <c r="R14" s="17"/>
+      <c r="S14" s="17"/>
+      <c r="T14" s="17"/>
+      <c r="U14" s="17"/>
+      <c r="V14" s="17"/>
+      <c r="W14" s="17"/>
+      <c r="X14" s="17"/>
+      <c r="Y14" s="17"/>
+      <c r="Z14" s="17"/>
+    </row>
+    <row r="15" spans="1:26" ht="19.5" customHeight="1">
+      <c r="A15" s="17"/>
+      <c r="B15" s="37"/>
+      <c r="C15" s="65" t="s">
+        <v>95</v>
+      </c>
+      <c r="D15" s="90" t="str">
+        <f>VLOOKUP(C10,'Formato descripción HU'!B6:O23,3,0)</f>
+        <v>Detectar retrasos y sancionar</v>
+      </c>
+      <c r="E15" s="70"/>
+      <c r="F15" s="27"/>
+      <c r="G15" s="65" t="s">
+        <v>96</v>
+      </c>
+      <c r="H15" s="90" t="str">
+        <f>VLOOKUP(C10,'Formato descripción HU'!B6:O23,4,0)</f>
+        <v>Fomentar uso responsable</v>
+      </c>
+      <c r="I15" s="69"/>
+      <c r="J15" s="70"/>
+      <c r="K15" s="27"/>
+      <c r="L15" s="65" t="s">
+        <v>97</v>
+      </c>
+      <c r="M15" s="68" t="str">
+        <f>VLOOKUP(C10,'Formato descripción HU'!B6:O23,6,0)</f>
+        <v>Registrar devolución → Detectar retraso → Notificar → Bloquear</v>
+      </c>
+      <c r="N15" s="69"/>
+      <c r="O15" s="70"/>
+      <c r="P15" s="38"/>
+      <c r="Q15" s="17"/>
+      <c r="R15" s="17"/>
+      <c r="S15" s="17"/>
+      <c r="T15" s="17"/>
+      <c r="U15" s="17"/>
+      <c r="V15" s="17"/>
+      <c r="W15" s="17"/>
+      <c r="X15" s="17"/>
+      <c r="Y15" s="17"/>
+      <c r="Z15" s="17"/>
+    </row>
+    <row r="16" spans="1:26" ht="19.5" customHeight="1">
+      <c r="A16" s="17"/>
+      <c r="B16" s="37"/>
+      <c r="C16" s="66"/>
+      <c r="D16" s="71"/>
+      <c r="E16" s="73"/>
+      <c r="F16" s="27"/>
+      <c r="G16" s="66"/>
+      <c r="H16" s="71"/>
+      <c r="I16" s="72"/>
+      <c r="J16" s="73"/>
+      <c r="K16" s="27"/>
+      <c r="L16" s="66"/>
+      <c r="M16" s="71"/>
+      <c r="N16" s="72"/>
+      <c r="O16" s="73"/>
+      <c r="P16" s="38"/>
+      <c r="Q16" s="17"/>
+      <c r="R16" s="17"/>
+      <c r="S16" s="17"/>
+      <c r="T16" s="17"/>
+      <c r="U16" s="17"/>
+      <c r="V16" s="17"/>
+      <c r="W16" s="17"/>
+      <c r="X16" s="17"/>
+      <c r="Y16" s="17"/>
+      <c r="Z16" s="17"/>
+    </row>
+    <row r="17" spans="1:26" ht="19.5" customHeight="1">
+      <c r="A17" s="17"/>
+      <c r="B17" s="37"/>
+      <c r="C17" s="67"/>
+      <c r="D17" s="74"/>
+      <c r="E17" s="76"/>
+      <c r="F17" s="27"/>
+      <c r="G17" s="67"/>
+      <c r="H17" s="74"/>
+      <c r="I17" s="75"/>
+      <c r="J17" s="76"/>
+      <c r="K17" s="27"/>
+      <c r="L17" s="67"/>
+      <c r="M17" s="74"/>
+      <c r="N17" s="75"/>
+      <c r="O17" s="76"/>
+      <c r="P17" s="38"/>
+      <c r="Q17" s="17"/>
+      <c r="R17" s="17"/>
+      <c r="S17" s="17"/>
+      <c r="T17" s="17"/>
+      <c r="U17" s="17"/>
+      <c r="V17" s="17"/>
+      <c r="W17" s="17"/>
+      <c r="X17" s="17"/>
+      <c r="Y17" s="17"/>
+      <c r="Z17" s="17"/>
+    </row>
+    <row r="18" spans="1:26" ht="9.75" customHeight="1">
+      <c r="A18" s="17"/>
+      <c r="B18" s="37"/>
+      <c r="C18" s="21"/>
+      <c r="D18" s="21"/>
+      <c r="E18" s="21"/>
+      <c r="F18" s="21"/>
+      <c r="G18" s="23"/>
+      <c r="H18" s="23"/>
+      <c r="I18" s="23"/>
+      <c r="J18" s="21"/>
+      <c r="K18" s="21"/>
+      <c r="L18" s="21"/>
+      <c r="M18" s="21"/>
+      <c r="N18" s="21"/>
+      <c r="O18" s="21"/>
+      <c r="P18" s="38"/>
+      <c r="Q18" s="17"/>
+      <c r="R18" s="17"/>
+      <c r="S18" s="17"/>
+      <c r="T18" s="17"/>
+      <c r="U18" s="17"/>
+      <c r="V18" s="17"/>
+      <c r="W18" s="17"/>
+      <c r="X18" s="17"/>
+      <c r="Y18" s="17"/>
+      <c r="Z18" s="17"/>
+    </row>
+    <row r="19" spans="1:26" ht="19.5" customHeight="1">
+      <c r="B19" s="37"/>
+      <c r="C19" s="85" t="s">
+        <v>98</v>
+      </c>
+      <c r="D19" s="70"/>
+      <c r="E19" s="77" t="str">
+        <f>VLOOKUP(C10,'Formato descripción HU'!B6:O23,14,0)</f>
+        <v>Sanciones automáticas</v>
+      </c>
+      <c r="F19" s="78"/>
+      <c r="G19" s="78"/>
+      <c r="H19" s="78"/>
+      <c r="I19" s="78"/>
+      <c r="J19" s="78"/>
+      <c r="K19" s="78"/>
+      <c r="L19" s="78"/>
+      <c r="M19" s="78"/>
+      <c r="N19" s="78"/>
+      <c r="O19" s="79"/>
+      <c r="P19" s="38"/>
+      <c r="Q19" s="17"/>
+    </row>
+    <row r="20" spans="1:26" ht="19.5" customHeight="1">
+      <c r="B20" s="37"/>
+      <c r="C20" s="74"/>
+      <c r="D20" s="76"/>
+      <c r="E20" s="80"/>
+      <c r="F20" s="81"/>
+      <c r="G20" s="81"/>
+      <c r="H20" s="81"/>
+      <c r="I20" s="81"/>
+      <c r="J20" s="81"/>
+      <c r="K20" s="81"/>
+      <c r="L20" s="81"/>
+      <c r="M20" s="81"/>
+      <c r="N20" s="81"/>
+      <c r="O20" s="82"/>
+      <c r="P20" s="38"/>
+      <c r="Q20" s="17"/>
+    </row>
+    <row r="21" spans="1:26" ht="9.75" customHeight="1">
+      <c r="B21" s="37"/>
+      <c r="C21" s="21"/>
+      <c r="D21" s="21"/>
+      <c r="E21" s="21"/>
+      <c r="F21" s="21"/>
+      <c r="G21" s="21"/>
+      <c r="H21" s="21"/>
+      <c r="I21" s="21"/>
+      <c r="J21" s="21"/>
+      <c r="K21" s="21"/>
+      <c r="L21" s="21"/>
+      <c r="M21" s="21"/>
+      <c r="N21" s="21"/>
+      <c r="O21" s="21"/>
+      <c r="P21" s="38"/>
+      <c r="Q21" s="17"/>
+    </row>
+    <row r="22" spans="1:26" ht="19.5" customHeight="1">
+      <c r="A22" s="17"/>
+      <c r="B22" s="37"/>
+      <c r="C22" s="86" t="s">
+        <v>99</v>
+      </c>
+      <c r="D22" s="70"/>
+      <c r="E22" s="87" t="str">
+        <f>VLOOKUP(C10,'Formato descripción HU'!B6:O23,12,0)</f>
+        <v>Al segundo retraso, bloquea usuario y notifica.</v>
+      </c>
+      <c r="F22" s="69"/>
+      <c r="G22" s="69"/>
+      <c r="H22" s="70"/>
+      <c r="I22" s="21"/>
+      <c r="J22" s="86" t="s">
+        <v>13</v>
+      </c>
+      <c r="K22" s="70"/>
+      <c r="L22" s="89" t="str">
+        <f>VLOOKUP(C10,'Formato descripción HU'!B6:O23,13,0)</f>
+        <v>Depende del historial</v>
+      </c>
+      <c r="M22" s="69"/>
+      <c r="N22" s="69"/>
+      <c r="O22" s="70"/>
+      <c r="P22" s="38"/>
+      <c r="Q22" s="17"/>
+      <c r="R22" s="17"/>
+      <c r="S22" s="17"/>
+      <c r="T22" s="17"/>
+      <c r="U22" s="17"/>
+      <c r="V22" s="17"/>
+      <c r="W22" s="17"/>
+      <c r="X22" s="17"/>
+      <c r="Y22" s="17"/>
+      <c r="Z22" s="17"/>
+    </row>
+    <row r="23" spans="1:26" ht="19.5" customHeight="1">
+      <c r="A23" s="17"/>
+      <c r="B23" s="37"/>
+      <c r="C23" s="71"/>
+      <c r="D23" s="73"/>
+      <c r="E23" s="71"/>
+      <c r="F23" s="72"/>
+      <c r="G23" s="72"/>
+      <c r="H23" s="73"/>
+      <c r="I23" s="21"/>
+      <c r="J23" s="71"/>
+      <c r="K23" s="73"/>
+      <c r="L23" s="71"/>
+      <c r="M23" s="72"/>
+      <c r="N23" s="72"/>
+      <c r="O23" s="73"/>
+      <c r="P23" s="38"/>
+      <c r="Q23" s="17"/>
+      <c r="R23" s="17"/>
+      <c r="S23" s="17"/>
+      <c r="T23" s="17"/>
+      <c r="U23" s="17"/>
+      <c r="V23" s="17"/>
+      <c r="W23" s="17"/>
+      <c r="X23" s="17"/>
+      <c r="Y23" s="17"/>
+      <c r="Z23" s="17"/>
+    </row>
+    <row r="24" spans="1:26" ht="19.5" customHeight="1">
+      <c r="A24" s="17"/>
+      <c r="B24" s="37"/>
+      <c r="C24" s="74"/>
+      <c r="D24" s="76"/>
+      <c r="E24" s="74"/>
+      <c r="F24" s="75"/>
+      <c r="G24" s="75"/>
+      <c r="H24" s="76"/>
+      <c r="I24" s="21"/>
+      <c r="J24" s="74"/>
+      <c r="K24" s="76"/>
+      <c r="L24" s="74"/>
+      <c r="M24" s="75"/>
+      <c r="N24" s="75"/>
+      <c r="O24" s="76"/>
       <c r="P24" s="38"/>
       <c r="Q24" s="17"/>
       <c r="R24" s="17"/>
@@ -34596,7 +36878,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{C7464F15-59D8-447C-B97A-3A303B371DF5}">
+        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{E42319A4-278D-44DA-BDA5-975495DCF500}">
           <x14:formula1>
             <xm:f>'Formato descripción HU'!$B$6:$B$23</xm:f>
           </x14:formula1>

</xml_diff>